<commit_message>
Updated with identifiers, and maps_to relationships random functions taken out because protoge won't load it
</commit_message>
<xml_diff>
--- a/EMFOConceptsAndRelationships.xlsx
+++ b/EMFOConceptsAndRelationships.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nih.sharepoint.com/sites/CC-RMD-Epidemiology-Biostatistics-Section/Shared Documents/Ontology/Product/Concepts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guydi\Downloads\Protege-5.6.3-win\Protege-5.6.3\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E6CC6E2-1069-4144-B1D6-3A9FE3E86982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF2955B-2A40-4D21-8948-490E6BC6ECFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2475" yWindow="20550" windowWidth="28770" windowHeight="15570" tabRatio="946" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25440" yWindow="18120" windowWidth="23100" windowHeight="11700" tabRatio="946" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="1" r:id="rId1"/>
-    <sheet name="Relations" sheetId="4" r:id="rId2"/>
-    <sheet name="Relationships" sheetId="2" r:id="rId3"/>
-    <sheet name="Technical Notes" sheetId="14" r:id="rId4"/>
+    <sheet name="Sources" sheetId="15" r:id="rId2"/>
+    <sheet name="Relations" sheetId="4" r:id="rId3"/>
+    <sheet name="Relationships" sheetId="2" r:id="rId4"/>
+    <sheet name="Technical Notes" sheetId="14" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="287">
   <si>
     <t>Ontology of Mental Functioning</t>
   </si>
@@ -198,9 +199,6 @@
   </si>
   <si>
     <t>Definition_Source</t>
-  </si>
-  <si>
-    <t>RID_00001</t>
   </si>
   <si>
     <t>provides_input_for</t>
@@ -400,6 +398,510 @@
   </si>
   <si>
     <t>is_a_non_anatomical_phenomenon_within</t>
+  </si>
+  <si>
+    <t>EMFO_C030990</t>
+  </si>
+  <si>
+    <t>EMFO_C051211</t>
+  </si>
+  <si>
+    <t>EMFO_C011176</t>
+  </si>
+  <si>
+    <t>EMFO_C013472</t>
+  </si>
+  <si>
+    <t>EMFO_C033547</t>
+  </si>
+  <si>
+    <t>EMFO_C067619</t>
+  </si>
+  <si>
+    <t>EMFO_C000677</t>
+  </si>
+  <si>
+    <t>EMFO_C052971</t>
+  </si>
+  <si>
+    <t>EMFO_C093989</t>
+  </si>
+  <si>
+    <t>EMFO_C053006</t>
+  </si>
+  <si>
+    <t>EMFO_C065492</t>
+  </si>
+  <si>
+    <t>EMFO_C047217</t>
+  </si>
+  <si>
+    <t>EMFO_C040176</t>
+  </si>
+  <si>
+    <t>EMFO_C007687</t>
+  </si>
+  <si>
+    <t>EMFO_C010942</t>
+  </si>
+  <si>
+    <t>EMFO_C015011</t>
+  </si>
+  <si>
+    <t>EMFO_C088043</t>
+  </si>
+  <si>
+    <t>EMFO_C015158</t>
+  </si>
+  <si>
+    <t>EMFO_C049286</t>
+  </si>
+  <si>
+    <t>EMFO_C056395</t>
+  </si>
+  <si>
+    <t>EMFO_C051998</t>
+  </si>
+  <si>
+    <t>EMFO_C024399</t>
+  </si>
+  <si>
+    <t>EMFO_C005547</t>
+  </si>
+  <si>
+    <t>EMFO_C022668</t>
+  </si>
+  <si>
+    <t>EMFO_C017617</t>
+  </si>
+  <si>
+    <t>EMFO_C022446</t>
+  </si>
+  <si>
+    <t>EMFO_C080772</t>
+  </si>
+  <si>
+    <t>EMFO_C039353</t>
+  </si>
+  <si>
+    <t>EMFO_C040767</t>
+  </si>
+  <si>
+    <t>EMFO_C017957</t>
+  </si>
+  <si>
+    <t>EMFO_C016694</t>
+  </si>
+  <si>
+    <t>EMFO_C012595</t>
+  </si>
+  <si>
+    <t>EMFO_C034733</t>
+  </si>
+  <si>
+    <t>EMFO_C030754</t>
+  </si>
+  <si>
+    <t>EMFO_C029787</t>
+  </si>
+  <si>
+    <t>EMFO_C088033</t>
+  </si>
+  <si>
+    <t>EMFO_C030067</t>
+  </si>
+  <si>
+    <t>EMFO_C030581</t>
+  </si>
+  <si>
+    <t>EMFO_C052832</t>
+  </si>
+  <si>
+    <t>EMFO_C042870</t>
+  </si>
+  <si>
+    <t>EMFO_C034289</t>
+  </si>
+  <si>
+    <t>EMFO_C018902</t>
+  </si>
+  <si>
+    <t>EMFO_C031158</t>
+  </si>
+  <si>
+    <t>EMFO_C078776</t>
+  </si>
+  <si>
+    <t>EMFO_C001285</t>
+  </si>
+  <si>
+    <t>EMFO_C074894</t>
+  </si>
+  <si>
+    <t>EMFO_C070087</t>
+  </si>
+  <si>
+    <t>EMFO_C071635</t>
+  </si>
+  <si>
+    <t>EMFO_C052559</t>
+  </si>
+  <si>
+    <t>EMFO_C016539</t>
+  </si>
+  <si>
+    <t>EMFO_C034816</t>
+  </si>
+  <si>
+    <t>EMFO_C076426</t>
+  </si>
+  <si>
+    <t>EMFO_C009564</t>
+  </si>
+  <si>
+    <t>EMFO_C068820</t>
+  </si>
+  <si>
+    <t>EMFO_C086955</t>
+  </si>
+  <si>
+    <t>EMFO_C038847</t>
+  </si>
+  <si>
+    <t>EMFO_C044109</t>
+  </si>
+  <si>
+    <t>EMFO_C094572</t>
+  </si>
+  <si>
+    <t>EMFO_C089159</t>
+  </si>
+  <si>
+    <t>EMFO_C024741</t>
+  </si>
+  <si>
+    <t>EMFO_C029317</t>
+  </si>
+  <si>
+    <t>Random No</t>
+  </si>
+  <si>
+    <t>EMFO_R00001</t>
+  </si>
+  <si>
+    <t>EMFO_R00002</t>
+  </si>
+  <si>
+    <t>EMFO_R00003</t>
+  </si>
+  <si>
+    <t>EMFO_R00004</t>
+  </si>
+  <si>
+    <t>EMFO_R00005</t>
+  </si>
+  <si>
+    <t>EMFO_R00006</t>
+  </si>
+  <si>
+    <t>EMFO_R00007</t>
+  </si>
+  <si>
+    <t>EMFO_R00008</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>EMFO_RS_0083451</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0287793</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0510569</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0368660</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0249384</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0823565</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0935376</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0052277</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0703280</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0937674</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0781704</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0978365</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0429648</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0822806</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0719807</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0662942</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0540418</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0203291</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0914762</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0153328</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0677980</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0346946</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0082542</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0910182</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0846653</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0573709</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0730902</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0565663</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0578882</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0192391</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0629834</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0307396</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0160780</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0972921</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0653465</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0322169</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0202981</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0722420</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0446992</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0874853</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0705129</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0507882</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0330342</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0086707</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0550539</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0415484</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0992572</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0717393</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0683021</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0156076</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0539662</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0771538</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0925311</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0009896</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0165453</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0714554</t>
+  </si>
+  <si>
+    <t>maps_to</t>
+  </si>
+  <si>
+    <t>Bodily_Process</t>
+  </si>
+  <si>
+    <t>bodily_process</t>
+  </si>
+  <si>
+    <t>OGMS_0000060</t>
+  </si>
+  <si>
+    <t>Source's Full Name</t>
+  </si>
+  <si>
+    <t>Source Abbrivation</t>
+  </si>
+  <si>
+    <t>Ontology for Genearl Medical Science</t>
+  </si>
+  <si>
+    <t>OGMS</t>
+  </si>
+  <si>
+    <t>RO</t>
+  </si>
+  <si>
+    <t>Basic Formal Ontology</t>
+  </si>
+  <si>
+    <t>BFO</t>
+  </si>
+  <si>
+    <t>Relation Ontology</t>
+  </si>
+  <si>
+    <t>EMFO</t>
+  </si>
+  <si>
+    <t>Ecological Mental Functioning Ontology</t>
+  </si>
+  <si>
+    <t>Rehabilitation Medicine Department, NIH Clinical Center</t>
+  </si>
+  <si>
+    <t>Ecological Model of Mental Functioning</t>
+  </si>
+  <si>
+    <t>SNOMED_CT</t>
+  </si>
+  <si>
+    <t>International Classification of Functioning, Disability and Health</t>
+  </si>
+  <si>
+    <t>EMFO_R00009</t>
+  </si>
+  <si>
+    <t>process</t>
+  </si>
+  <si>
+    <t>OGMS_0000087</t>
+  </si>
+  <si>
+    <t>independent continuant</t>
+  </si>
+  <si>
+    <t>BFO_0000004</t>
+  </si>
+  <si>
+    <t>continuant</t>
+  </si>
+  <si>
+    <t>mental_functioning_related_anitomical_structures</t>
+  </si>
+  <si>
+    <t>mental process</t>
+  </si>
+  <si>
+    <t>MFO</t>
+  </si>
+  <si>
+    <t>Mental Functioning Ontology (Jenna Hastings)</t>
+  </si>
+  <si>
+    <t>bodily process</t>
+  </si>
+  <si>
+    <t>MF_0000000</t>
+  </si>
+  <si>
+    <t>GO</t>
+  </si>
+  <si>
+    <t>GO_0007610</t>
+  </si>
+  <si>
+    <t>Gene Ontology</t>
+  </si>
+  <si>
+    <t>MF_0000020</t>
+  </si>
+  <si>
+    <t>extended organism</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0319446</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0649787</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0013391</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0112714</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0158156</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0971284</t>
   </si>
 </sst>
 </file>
@@ -584,7 +1086,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="42">
+  <fills count="43">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -818,6 +1320,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -994,7 +1502,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1028,6 +1536,7 @@
     <xf numFmtId="0" fontId="0" fillId="41" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="41" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="41" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1079,11 +1588,11 @@
   </tableStyles>
   <colors>
     <mruColors>
-      <color rgb="FFFFD6C1"/>
       <color rgb="FFFFCFB7"/>
-      <color rgb="FFFFCC99"/>
       <color rgb="FFF0D9FF"/>
       <color rgb="FFCE85FF"/>
+      <color rgb="FFFFD6C1"/>
+      <color rgb="FFFFCC99"/>
       <color rgb="FFD9F0C8"/>
     </mruColors>
   </colors>
@@ -1395,25 +1904,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView topLeftCell="B47" zoomScale="226" zoomScaleNormal="226" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.140625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" style="4" customWidth="1"/>
     <col min="2" max="2" width="42" style="4" customWidth="1"/>
     <col min="3" max="3" width="32.5703125" style="4" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" style="4" customWidth="1"/>
     <col min="5" max="6" width="15.28515625" style="4" customWidth="1"/>
     <col min="7" max="7" width="19.85546875" style="4" customWidth="1"/>
     <col min="8" max="8" width="23.5703125" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="4"/>
+    <col min="9" max="9" width="19.42578125" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -1427,7 +1937,7 @@
         <v>52</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>53</v>
@@ -1436,18 +1946,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>0</v>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>149</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D2" s="4">
-        <v>100</v>
+        <v>6</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>8</v>
@@ -1456,10 +1966,10 @@
         <v>8</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>30</v>
       </c>
@@ -1469,8 +1979,14 @@
       <c r="C3" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>31</v>
       </c>
@@ -1480,8 +1996,14 @@
       <c r="C4" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D4" s="4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>32</v>
       </c>
@@ -1491,10 +2013,16 @@
       <c r="C5" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="D5" s="4">
         <v>1</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>150</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>27</v>
@@ -1502,10 +2030,16 @@
       <c r="C6" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>2</v>
+      <c r="D6" s="4">
+        <v>4</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>151</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>1</v>
@@ -1514,8 +2048,7 @@
         <v>26</v>
       </c>
       <c r="D7" s="5">
-        <f>D2+1</f>
-        <v>101</v>
+        <v>4</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>9</v>
@@ -1524,22 +2057,22 @@
         <v>9</v>
       </c>
       <c r="G7" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>3</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>63</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D8" s="5">
-        <f t="shared" ref="D8:D21" si="0">D7+1</f>
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>7</v>
@@ -1548,22 +2081,22 @@
         <v>7</v>
       </c>
       <c r="G8" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>4</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>65</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>28</v>
       </c>
       <c r="D9" s="5">
-        <f t="shared" si="0"/>
-        <v>103</v>
+        <v>7</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>10</v>
@@ -1572,30 +2105,34 @@
         <v>10</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>121</v>
+      </c>
       <c r="B10" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>5</v>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>122</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D11" s="5">
-        <f>D9+1</f>
-        <v>104</v>
+        <v>7</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>10</v>
@@ -1604,22 +2141,22 @@
         <v>10</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
-        <v>6</v>
+        <v>67</v>
+      </c>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>123</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D12" s="5">
-        <f t="shared" si="0"/>
-        <v>105</v>
+        <v>7</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>10</v>
@@ -1628,22 +2165,22 @@
         <v>10</v>
       </c>
       <c r="G12" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
-        <v>7</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D13" s="5">
-        <f t="shared" si="0"/>
-        <v>106</v>
+        <v>8</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>7</v>
@@ -1652,22 +2189,22 @@
         <v>7</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
-        <v>8</v>
+        <v>67</v>
+      </c>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>125</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="5">
-        <f t="shared" si="0"/>
-        <v>107</v>
+        <v>7</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>10</v>
@@ -1676,22 +2213,22 @@
         <v>10</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
-        <v>9</v>
+        <v>67</v>
+      </c>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>126</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D15" s="5">
-        <f t="shared" si="0"/>
-        <v>108</v>
+        <v>7</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>10</v>
@@ -1700,22 +2237,22 @@
         <v>10</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
-        <v>10</v>
+        <v>67</v>
+      </c>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>127</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="5">
-        <f t="shared" si="0"/>
-        <v>109</v>
+        <v>7</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>10</v>
@@ -1724,22 +2261,22 @@
         <v>10</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
-        <v>11</v>
+        <v>67</v>
+      </c>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>128</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="5">
-        <f t="shared" si="0"/>
-        <v>110</v>
+        <v>7</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>10</v>
@@ -1748,22 +2285,22 @@
         <v>10</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
-        <v>12</v>
+        <v>67</v>
+      </c>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>129</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="5">
-        <f t="shared" si="0"/>
-        <v>111</v>
+        <v>7</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>10</v>
@@ -1772,22 +2309,22 @@
         <v>10</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
-        <v>13</v>
+        <v>67</v>
+      </c>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>130</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="5">
-        <f t="shared" si="0"/>
-        <v>112</v>
+        <v>7</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>10</v>
@@ -1796,22 +2333,22 @@
         <v>10</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
-        <v>14</v>
+        <v>67</v>
+      </c>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="5">
-        <f t="shared" si="0"/>
-        <v>113</v>
+        <v>7</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>10</v>
@@ -1820,22 +2357,22 @@
         <v>10</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
-        <v>15</v>
+        <v>67</v>
+      </c>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>132</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D21" s="5">
-        <f t="shared" si="0"/>
-        <v>114</v>
+        <v>7</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>10</v>
@@ -1844,62 +2381,100 @@
         <v>10</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>133</v>
+      </c>
       <c r="B22" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:8" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B23" s="8" t="s">
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="1:8" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B26" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>138</v>
+      </c>
       <c r="B27" s="6" t="s">
         <v>37</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>25</v>
       </c>
+      <c r="D27" s="6">
+        <v>7</v>
+      </c>
       <c r="E27" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>139</v>
+      </c>
       <c r="B28" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>140</v>
+      </c>
       <c r="B29" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
+      </c>
+      <c r="D29" s="6">
+        <v>7</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>10</v>
@@ -1907,281 +2482,567 @@
       <c r="F29" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>141</v>
+      </c>
       <c r="B30" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>142</v>
+      </c>
       <c r="B31" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H31" s="4"/>
+    </row>
+    <row r="32" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C31" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="6" t="s">
-        <v>86</v>
-      </c>
       <c r="C32" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="H32" s="4"/>
+    </row>
+    <row r="33" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>144</v>
+      </c>
       <c r="B33" s="6" t="s">
         <v>41</v>
       </c>
+      <c r="D33" s="6">
+        <v>4</v>
+      </c>
       <c r="E33" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="34" spans="2:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H33" s="4"/>
+    </row>
+    <row r="34" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>145</v>
+      </c>
       <c r="B34" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C34" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="H34" s="4"/>
+    </row>
+    <row r="35" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="35" spans="2:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="6" t="s">
-        <v>87</v>
-      </c>
       <c r="C35" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
+      </c>
+      <c r="D35" s="6">
+        <v>7</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="2:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H35" s="4"/>
+    </row>
+    <row r="36" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>147</v>
+      </c>
       <c r="B36" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
+      </c>
+      <c r="D36" s="6">
+        <v>7</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="37" spans="2:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H36" s="4"/>
+    </row>
+    <row r="37" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>148</v>
+      </c>
       <c r="B37" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C37" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B38" s="6" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="38" spans="2:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="6" t="s">
-        <v>91</v>
-      </c>
       <c r="C38" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
+      </c>
+      <c r="D38" s="6">
+        <v>4</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="39" spans="2:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H38" s="4"/>
+    </row>
+    <row r="39" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>153</v>
+      </c>
       <c r="B39" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
+      </c>
+      <c r="D39" s="6">
+        <v>7</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="40" spans="2:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>154</v>
+      </c>
       <c r="B40" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
+      </c>
+      <c r="D40" s="6">
+        <v>7</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="41" spans="2:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>155</v>
+      </c>
       <c r="B41" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
+      </c>
+      <c r="D41" s="6">
+        <v>4</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="42" spans="2:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>156</v>
+      </c>
       <c r="B42" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
+      </c>
+      <c r="D42" s="6">
+        <v>4</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="43" spans="2:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>157</v>
+      </c>
       <c r="B43" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
+      </c>
+      <c r="D43" s="6">
+        <v>4</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="44" spans="2:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>158</v>
+      </c>
       <c r="B44" s="6" t="s">
         <v>45</v>
       </c>
+      <c r="D44" s="6">
+        <v>7</v>
+      </c>
       <c r="E44" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="45" spans="2:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H44" s="4"/>
+    </row>
+    <row r="45" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>159</v>
+      </c>
       <c r="B45" s="6" t="s">
         <v>46</v>
       </c>
+      <c r="D45" s="6">
+        <v>4</v>
+      </c>
       <c r="E45" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="46" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
+        <v>160</v>
+      </c>
       <c r="B46" s="7" t="s">
         <v>47</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="47" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H46" s="4"/>
+    </row>
+    <row r="47" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
+        <v>161</v>
+      </c>
       <c r="B47" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="48" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H47" s="4"/>
+    </row>
+    <row r="48" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
+        <v>162</v>
+      </c>
       <c r="B48" s="7" t="s">
         <v>48</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="H48" s="4"/>
+    </row>
+    <row r="49" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="7" t="s">
+        <v>163</v>
+      </c>
       <c r="B49" s="7" t="s">
         <v>49</v>
       </c>
       <c r="C49" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="H49" s="4"/>
+    </row>
+    <row r="50" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B50" s="7" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="50" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="7" t="s">
+      <c r="H50" s="4"/>
+    </row>
+    <row r="51" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="B51" s="7" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="51" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="7" t="s">
+      <c r="C51" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="H51" s="4"/>
+    </row>
+    <row r="52" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B52" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="C51" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="7" t="s">
+      <c r="H52" s="4"/>
+    </row>
+    <row r="53" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="B53" s="7" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="53" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="7" t="s">
+      <c r="H53" s="4"/>
+    </row>
+    <row r="54" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="B54" s="7" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="54" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="7" t="s">
+      <c r="H54" s="4"/>
+    </row>
+    <row r="55" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="B55" s="7" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="55" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="7" t="s">
+      <c r="H55" s="4"/>
+    </row>
+    <row r="56" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B56" s="7" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="56" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="7" t="s">
+      <c r="H56" s="4"/>
+    </row>
+    <row r="57" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B57" s="7" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="57" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="7" t="s">
+      <c r="H57" s="4"/>
+    </row>
+    <row r="58" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="B58" s="7" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="58" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="7" t="s">
+      <c r="H58" s="4"/>
+    </row>
+    <row r="59" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B59" s="7" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="59" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="7" t="s">
+      <c r="H59" s="4"/>
+    </row>
+    <row r="60" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="B60" s="7" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="60" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="7" t="s">
+      <c r="H60" s="4"/>
+    </row>
+    <row r="61" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="B61" s="7" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="61" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="7" t="s">
+      <c r="H61" s="4"/>
+    </row>
+    <row r="62" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B62" s="7" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="62" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="7" t="s">
+      <c r="H62" s="4"/>
+    </row>
+    <row r="63" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="B63" s="12" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="63" spans="2:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="12" t="s">
-        <v>110</v>
+      <c r="D63" s="12">
+        <v>4</v>
       </c>
       <c r="E63" s="12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="64" spans="2:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H63" s="4"/>
+    </row>
+    <row r="64" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="B64" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="D64" s="12">
+        <v>4</v>
       </c>
       <c r="E64" s="12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="65" spans="2:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H64" s="4"/>
+    </row>
+    <row r="65" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="12" t="s">
+        <v>179</v>
+      </c>
       <c r="B65" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
+      </c>
+      <c r="D65" s="12">
+        <v>4</v>
       </c>
       <c r="E65" s="12" t="s">
         <v>9</v>
+      </c>
+      <c r="H65" s="4"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="D67" s="4">
+        <v>3</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="D69" s="4">
+        <v>1</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="B70" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="D70" s="4">
+        <v>9</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="B71" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D71" s="4">
+        <v>10</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="B72" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D72" s="4">
+        <v>9</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -2190,11 +3051,152 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBC84FB6-CA19-4234-BB2F-E661E09ED822}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="62" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>250</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B3" t="s">
+        <v>254</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>252</v>
+      </c>
+      <c r="B4" t="s">
+        <v>253</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>261</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>259</v>
+      </c>
+      <c r="B6" t="s">
+        <v>258</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>260</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>263</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>262</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>273</v>
+      </c>
+      <c r="B10" t="s">
+        <v>272</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>278</v>
+      </c>
+      <c r="B11" t="s">
+        <v>276</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D798B18-C5BD-476F-9FF2-CDB45434B078}">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2209,22 +3211,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>116</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2239,30 +3241,45 @@
       <c r="A3" t="s">
         <v>17</v>
       </c>
+      <c r="B3" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
+      <c r="B4" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
+      <c r="B5" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>51</v>
       </c>
+      <c r="B6" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="B7" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
@@ -2270,20 +3287,37 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>117</v>
+        <v>116</v>
+      </c>
+      <c r="B9" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
+      <c r="B10" t="s">
+        <v>187</v>
+      </c>
       <c r="F10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>119</v>
+        <v>118</v>
+      </c>
+      <c r="B11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>246</v>
+      </c>
+      <c r="B12" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2299,25 +3333,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B15F685-1533-4446-BC92-30DBE05F964F}">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:F67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="E2" sqref="E2:F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" style="4" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" style="4" customWidth="1"/>
     <col min="2" max="2" width="31.28515625" style="10" customWidth="1"/>
     <col min="3" max="3" width="37.5703125" style="11" customWidth="1"/>
     <col min="4" max="4" width="44.85546875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="23" style="4" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>33</v>
@@ -2328,35 +3364,49 @@
       <c r="D1" s="13" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>54</v>
+        <v>190</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>34</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
+        <v>66</v>
+      </c>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+    </row>
+    <row r="3" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>191</v>
+      </c>
       <c r="B3" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>34</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
+        <v>66</v>
+      </c>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>192</v>
+      </c>
       <c r="B4" s="15" t="s">
         <v>1</v>
       </c>
@@ -2364,11 +3414,15 @@
         <v>34</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
+        <v>59</v>
+      </c>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+    </row>
+    <row r="5" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>193</v>
+      </c>
       <c r="B5" s="15" t="s">
         <v>1</v>
       </c>
@@ -2378,141 +3432,194 @@
       <c r="D5" s="15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+    </row>
+    <row r="6" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>194</v>
+      </c>
       <c r="B6" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>34</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
+        <v>69</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>195</v>
+      </c>
       <c r="B7" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>34</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
+        <v>70</v>
+      </c>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>196</v>
+      </c>
       <c r="B8" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>34</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
+        <v>71</v>
+      </c>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>197</v>
+      </c>
       <c r="B9" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>34</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
+        <v>72</v>
+      </c>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+    </row>
+    <row r="10" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>198</v>
+      </c>
       <c r="B10" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>34</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
+        <v>73</v>
+      </c>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+    </row>
+    <row r="11" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>199</v>
+      </c>
       <c r="B11" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>34</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
+        <v>74</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+    </row>
+    <row r="12" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>200</v>
+      </c>
       <c r="B12" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>34</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
+        <v>75</v>
+      </c>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+    </row>
+    <row r="13" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>201</v>
+      </c>
       <c r="B13" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>34</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
+        <v>76</v>
+      </c>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+    </row>
+    <row r="14" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>202</v>
+      </c>
       <c r="B14" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>34</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
+        <v>77</v>
+      </c>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+    </row>
+    <row r="15" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>203</v>
+      </c>
       <c r="B15" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>34</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
+        <v>77</v>
+      </c>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+    </row>
+    <row r="16" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>204</v>
+      </c>
       <c r="B16" s="15" t="s">
         <v>2</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>205</v>
+      </c>
       <c r="B18" s="19" t="s">
         <v>37</v>
       </c>
@@ -2522,155 +3629,207 @@
       <c r="D18" s="19" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="18"/>
+    </row>
+    <row r="19" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="18" t="s">
+        <v>206</v>
+      </c>
       <c r="B19" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C19" s="20" t="s">
         <v>34</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
+        <v>82</v>
+      </c>
+      <c r="E19" s="14"/>
+      <c r="F19" s="18"/>
+    </row>
+    <row r="20" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
+        <v>207</v>
+      </c>
       <c r="B20" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C20" s="20" t="s">
         <v>34</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
+        <v>82</v>
+      </c>
+      <c r="E20" s="14"/>
+      <c r="F20" s="18"/>
+    </row>
+    <row r="21" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="18" t="s">
+        <v>208</v>
+      </c>
       <c r="B21" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C21" s="20" t="s">
         <v>34</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
+        <v>82</v>
+      </c>
+      <c r="E21" s="14"/>
+      <c r="F21" s="18"/>
+    </row>
+    <row r="22" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="s">
+        <v>209</v>
+      </c>
       <c r="B22" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C22" s="20" t="s">
         <v>34</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
+        <v>82</v>
+      </c>
+      <c r="E22" s="14"/>
+      <c r="F22" s="18"/>
+    </row>
+    <row r="23" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="18" t="s">
+        <v>210</v>
+      </c>
       <c r="B23" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C23" s="20" t="s">
         <v>34</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
+        <v>84</v>
+      </c>
+      <c r="E23" s="14"/>
+      <c r="F23" s="18"/>
+    </row>
+    <row r="24" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="18" t="s">
+        <v>211</v>
+      </c>
       <c r="B24" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C24" s="20" t="s">
         <v>34</v>
       </c>
       <c r="D24" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" s="14"/>
+      <c r="F24" s="18"/>
+    </row>
+    <row r="25" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="B25" s="19" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
-      <c r="B25" s="19" t="s">
-        <v>91</v>
       </c>
       <c r="C25" s="20" t="s">
         <v>34</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
+        <v>88</v>
+      </c>
+      <c r="E25" s="14"/>
+      <c r="F25" s="18"/>
+    </row>
+    <row r="26" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="18" t="s">
+        <v>213</v>
+      </c>
       <c r="B26" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C26" s="20" t="s">
         <v>34</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="18"/>
+        <v>89</v>
+      </c>
+      <c r="E26" s="14"/>
+      <c r="F26" s="18"/>
+    </row>
+    <row r="27" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="18" t="s">
+        <v>214</v>
+      </c>
       <c r="B27" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C27" s="20" t="s">
         <v>34</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
+        <v>84</v>
+      </c>
+      <c r="E27" s="14"/>
+      <c r="F27" s="18"/>
+    </row>
+    <row r="28" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="18" t="s">
+        <v>215</v>
+      </c>
       <c r="B28" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C28" s="20" t="s">
         <v>34</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
+        <v>86</v>
+      </c>
+      <c r="E28" s="14"/>
+      <c r="F28" s="18"/>
+    </row>
+    <row r="29" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="18" t="s">
+        <v>216</v>
+      </c>
       <c r="B29" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C29" s="20" t="s">
         <v>34</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
+        <v>86</v>
+      </c>
+      <c r="E29" s="14"/>
+      <c r="F29" s="18"/>
+    </row>
+    <row r="30" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="18" t="s">
+        <v>217</v>
+      </c>
       <c r="B30" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C30" s="20" t="s">
         <v>34</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
+        <v>86</v>
+      </c>
+      <c r="E30" s="14"/>
+      <c r="F30" s="18"/>
+    </row>
+    <row r="31" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="18" t="s">
+        <v>218</v>
+      </c>
       <c r="B31" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C31" s="20" t="s">
         <v>34</v>
@@ -2678,9 +3837,13 @@
       <c r="D31" s="19" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="18"/>
+    </row>
+    <row r="32" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="18" t="s">
+        <v>219</v>
+      </c>
       <c r="B32" s="18" t="s">
         <v>41</v>
       </c>
@@ -2690,9 +3853,13 @@
       <c r="D32" s="18" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="18"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="18"/>
+    </row>
+    <row r="33" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="18" t="s">
+        <v>220</v>
+      </c>
       <c r="B33" s="19" t="s">
         <v>41</v>
       </c>
@@ -2702,9 +3869,13 @@
       <c r="D33" s="19" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="18"/>
+    </row>
+    <row r="34" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="18" t="s">
+        <v>221</v>
+      </c>
       <c r="B34" s="19" t="s">
         <v>41</v>
       </c>
@@ -2714,9 +3885,13 @@
       <c r="D34" s="19" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="18"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="18"/>
+    </row>
+    <row r="35" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="18" t="s">
+        <v>222</v>
+      </c>
       <c r="B35" s="18" t="s">
         <v>41</v>
       </c>
@@ -2726,9 +3901,13 @@
       <c r="D35" s="18" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="18"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="18"/>
+    </row>
+    <row r="36" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="18" t="s">
+        <v>223</v>
+      </c>
       <c r="B36" s="19" t="s">
         <v>39</v>
       </c>
@@ -2738,9 +3917,13 @@
       <c r="D36" s="19" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="18"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="18"/>
+    </row>
+    <row r="37" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="18" t="s">
+        <v>224</v>
+      </c>
       <c r="B37" s="18" t="s">
         <v>46</v>
       </c>
@@ -2750,9 +3933,13 @@
       <c r="D37" s="18" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="18"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="18"/>
+    </row>
+    <row r="38" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="18" t="s">
+        <v>225</v>
+      </c>
       <c r="B38" s="19" t="s">
         <v>43</v>
       </c>
@@ -2762,9 +3949,18 @@
       <c r="D38" s="19" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="22"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="18"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="22" t="s">
+        <v>226</v>
+      </c>
       <c r="B40" s="23" t="s">
         <v>47</v>
       </c>
@@ -2774,9 +3970,13 @@
       <c r="D40" s="23" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="22"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="22"/>
+    </row>
+    <row r="41" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="22" t="s">
+        <v>227</v>
+      </c>
       <c r="B41" s="23" t="s">
         <v>47</v>
       </c>
@@ -2784,11 +3984,15 @@
         <v>34</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="22"/>
+        <v>59</v>
+      </c>
+      <c r="E41" s="14"/>
+      <c r="F41" s="22"/>
+    </row>
+    <row r="42" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="22" t="s">
+        <v>228</v>
+      </c>
       <c r="B42" s="23" t="s">
         <v>48</v>
       </c>
@@ -2796,11 +4000,15 @@
         <v>34</v>
       </c>
       <c r="D42" s="23" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="22"/>
+        <v>95</v>
+      </c>
+      <c r="E42" s="14"/>
+      <c r="F42" s="22"/>
+    </row>
+    <row r="43" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="22" t="s">
+        <v>229</v>
+      </c>
       <c r="B43" s="23" t="s">
         <v>49</v>
       </c>
@@ -2808,145 +4016,198 @@
         <v>34</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="22"/>
+        <v>95</v>
+      </c>
+      <c r="E43" s="14"/>
+      <c r="F43" s="22"/>
+    </row>
+    <row r="44" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="22" t="s">
+        <v>230</v>
+      </c>
       <c r="B44" s="23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C44" s="24" t="s">
         <v>34</v>
       </c>
       <c r="D44" s="23" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="22"/>
+        <v>97</v>
+      </c>
+      <c r="E44" s="14"/>
+      <c r="F44" s="22"/>
+    </row>
+    <row r="45" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="22" t="s">
+        <v>231</v>
+      </c>
       <c r="B45" s="23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C45" s="24" t="s">
         <v>34</v>
       </c>
       <c r="D45" s="23" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="22"/>
+        <v>97</v>
+      </c>
+      <c r="E45" s="14"/>
+      <c r="F45" s="22"/>
+    </row>
+    <row r="46" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="22" t="s">
+        <v>232</v>
+      </c>
       <c r="B46" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C46" s="24" t="s">
         <v>34</v>
       </c>
       <c r="D46" s="23" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="22"/>
+        <v>97</v>
+      </c>
+      <c r="E46" s="14"/>
+      <c r="F46" s="22"/>
+    </row>
+    <row r="47" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="22" t="s">
+        <v>233</v>
+      </c>
       <c r="B47" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C47" s="24" t="s">
         <v>34</v>
       </c>
       <c r="D47" s="23" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="22"/>
+        <v>97</v>
+      </c>
+      <c r="E47" s="14"/>
+      <c r="F47" s="22"/>
+    </row>
+    <row r="48" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="22" t="s">
+        <v>234</v>
+      </c>
       <c r="B48" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C48" s="24" t="s">
         <v>34</v>
       </c>
       <c r="D48" s="23" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="22"/>
+        <v>96</v>
+      </c>
+      <c r="E48" s="14"/>
+      <c r="F48" s="22"/>
+    </row>
+    <row r="49" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="22" t="s">
+        <v>235</v>
+      </c>
       <c r="B49" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C49" s="24" t="s">
         <v>34</v>
       </c>
       <c r="D49" s="23" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="22"/>
+        <v>102</v>
+      </c>
+      <c r="E49" s="14"/>
+      <c r="F49" s="22"/>
+    </row>
+    <row r="50" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="22" t="s">
+        <v>236</v>
+      </c>
       <c r="B50" s="23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C50" s="24" t="s">
         <v>34</v>
       </c>
       <c r="D50" s="23" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="22"/>
+        <v>102</v>
+      </c>
+      <c r="E50" s="14"/>
+      <c r="F50" s="22"/>
+    </row>
+    <row r="51" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="22" t="s">
+        <v>237</v>
+      </c>
       <c r="B51" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C51" s="24" t="s">
         <v>34</v>
       </c>
       <c r="D51" s="23" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="22"/>
+        <v>102</v>
+      </c>
+      <c r="E51" s="14"/>
+      <c r="F51" s="22"/>
+    </row>
+    <row r="52" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="22" t="s">
+        <v>238</v>
+      </c>
       <c r="B52" s="23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C52" s="24" t="s">
         <v>34</v>
       </c>
       <c r="D52" s="23" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="22"/>
+        <v>106</v>
+      </c>
+      <c r="E52" s="14"/>
+      <c r="F52" s="22"/>
+    </row>
+    <row r="53" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="22" t="s">
+        <v>239</v>
+      </c>
       <c r="B53" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C53" s="24" t="s">
         <v>34</v>
       </c>
       <c r="D53" s="23" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="28"/>
+        <v>106</v>
+      </c>
+      <c r="E53" s="14"/>
+      <c r="F53" s="22"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="28" t="s">
+        <v>240</v>
+      </c>
       <c r="B55" s="29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C55" s="30" t="s">
         <v>34</v>
       </c>
       <c r="D55" s="29" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="28"/>
+        <v>59</v>
+      </c>
+      <c r="E55" s="14"/>
+      <c r="F55" s="28"/>
+    </row>
+    <row r="56" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="28" t="s">
+        <v>241</v>
+      </c>
       <c r="B56" s="29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C56" s="30" t="s">
         <v>34</v>
@@ -2954,11 +4215,15 @@
       <c r="D56" s="29" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="28"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="28"/>
+    </row>
+    <row r="57" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="28" t="s">
+        <v>242</v>
+      </c>
       <c r="B57" s="29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C57" s="30" t="s">
         <v>34</v>
@@ -2966,11 +4231,15 @@
       <c r="D57" s="29" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="28"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="28"/>
+    </row>
+    <row r="58" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="28" t="s">
+        <v>243</v>
+      </c>
       <c r="B58" s="29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C58" s="30" t="s">
         <v>34</v>
@@ -2978,11 +4247,15 @@
       <c r="D58" s="29" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="28"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="28"/>
+    </row>
+    <row r="59" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="28" t="s">
+        <v>244</v>
+      </c>
       <c r="B59" s="29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C59" s="30" t="s">
         <v>34</v>
@@ -2990,18 +4263,114 @@
       <c r="D59" s="29" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="28"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="28"/>
+    </row>
+    <row r="60" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="28" t="s">
+        <v>245</v>
+      </c>
       <c r="B60" s="29" t="s">
         <v>50</v>
       </c>
       <c r="C60" s="30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D60" s="29" t="s">
         <v>47</v>
       </c>
+      <c r="E60" s="14"/>
+      <c r="F60" s="28"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C62" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E62" s="14"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C63" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="E63" s="14"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C64" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="E64" s="14"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C65" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="D65" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="E65" s="14"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C66" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="D66" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E66" s="14"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C67" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="D67" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="E67" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3009,7 +4378,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F53A5C-C61C-46C4-AC07-17A8415AFB31}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3024,15 +4393,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="0c85289e-a0a4-4193-8a36-83840327cccf" xsi:nil="true"/>
@@ -3041,6 +4401,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3299,14 +4668,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4B4AC16-F988-4D41-8F01-205FCE01B916}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{084C8915-1C39-4800-8751-2F69F55F51E7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -3319,6 +4680,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="0c85289e-a0a4-4193-8a36-83840327cccf"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4B4AC16-F988-4D41-8F01-205FCE01B916}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
sooo many fixes.  Changed the root concept from ontology of mental functioning to ecological mental functioning ontology fixed space, punctuation and hyphen issues added maps to to the BasicEcologicalMentalFunctioningOntology.owl took out obsolete rules in the json file ran cellfie on the updated excel file and saved as EMFOwithoutRelationships.owl
</commit_message>
<xml_diff>
--- a/EMFOConceptsAndRelationships.xlsx
+++ b/EMFOConceptsAndRelationships.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guydi\Downloads\Protege-5.6.3-win\Protege-5.6.3\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\softwareRepos\EcologicalMentalFunctioningOntology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF2955B-2A40-4D21-8948-490E6BC6ECFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6187FF8-A250-41D9-A3C3-434C7A958046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25440" yWindow="18120" windowWidth="23100" windowHeight="11700" tabRatio="946" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="3420" windowWidth="23100" windowHeight="11700" tabRatio="946" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="1" r:id="rId1"/>
@@ -37,10 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="287">
-  <si>
-    <t>Ontology of Mental Functioning</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="286">
   <si>
     <t>Output</t>
   </si>
@@ -216,9 +213,6 @@
     <t>Imported_From</t>
   </si>
   <si>
-    <t>Ontology_of_Mental_Functioning</t>
-  </si>
-  <si>
     <t>Some_Definition1</t>
   </si>
   <si>
@@ -273,22 +267,12 @@
     <t>General_Tasks_and_Demands</t>
   </si>
   <si>
-    <t>Alone_or_with_others
-Requires_set-up
-Level_of_stress</t>
-  </si>
-  <si>
     <t>Mental_Activity_Demands</t>
   </si>
   <si>
     <t>Mental_Nature_of_Task</t>
   </si>
   <si>
-    <t>Simple_to_complex
-Temporal_–_brief_or_sustained
-Single_or_multiple_</t>
-  </si>
-  <si>
     <t>Person_Factors</t>
   </si>
   <si>
@@ -784,9 +768,6 @@
     <t>maps_to</t>
   </si>
   <si>
-    <t>Bodily_Process</t>
-  </si>
-  <si>
     <t>bodily_process</t>
   </si>
   <si>
@@ -902,6 +883,18 @@
   </si>
   <si>
     <t>EMFO_RS_0971284</t>
+  </si>
+  <si>
+    <t>extended_organism</t>
+  </si>
+  <si>
+    <t>Simple_to_complex_Temporal_brief_or_sustained_Single_or_multiple</t>
+  </si>
+  <si>
+    <t>Alone_or_with_others_Requires_set-up_Level_of_stress</t>
+  </si>
+  <si>
+    <t>Ecological_Mental_Functioning_Ontology</t>
   </si>
 </sst>
 </file>
@@ -1906,14 +1899,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="42" style="4" customWidth="1"/>
+    <col min="2" max="2" width="66.28515625" style="4" customWidth="1"/>
     <col min="3" max="3" width="32.5703125" style="4" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" style="4" customWidth="1"/>
     <col min="5" max="6" width="15.28515625" style="4" customWidth="1"/>
@@ -1925,1124 +1918,1124 @@
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>59</v>
+        <v>285</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2" s="4">
         <v>6</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="4">
         <v>1</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="D6" s="4">
         <v>4</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="5">
         <v>4</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="5">
         <v>8</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" s="5">
         <v>7</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" s="5">
         <v>7</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D12" s="5">
         <v>7</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D13" s="5">
         <v>8</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D14" s="5">
         <v>7</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D15" s="5">
         <v>7</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D16" s="5">
         <v>7</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D17" s="5">
         <v>7</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18" s="5">
         <v>7</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H18" s="4"/>
     </row>
     <row r="19" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D19" s="5">
         <v>7</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H19" s="4"/>
     </row>
     <row r="20" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D20" s="5">
         <v>7</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H20" s="4"/>
     </row>
     <row r="21" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D21" s="5">
         <v>7</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H21" s="4"/>
     </row>
     <row r="22" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" spans="1:8" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>78</v>
+        <v>284</v>
       </c>
       <c r="H23" s="4"/>
     </row>
     <row r="24" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H24" s="4"/>
     </row>
     <row r="25" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H25" s="4"/>
     </row>
-    <row r="26" spans="1:8" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>81</v>
+        <v>283</v>
       </c>
       <c r="H26" s="4"/>
     </row>
     <row r="27" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D27" s="6">
         <v>7</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H27" s="4"/>
     </row>
     <row r="28" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H28" s="4"/>
     </row>
     <row r="29" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D29" s="6">
         <v>7</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H29" s="4"/>
     </row>
     <row r="30" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H30" s="4"/>
     </row>
     <row r="31" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H31" s="4"/>
     </row>
     <row r="32" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H32" s="4"/>
     </row>
     <row r="33" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D33" s="6">
         <v>4</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H33" s="4"/>
     </row>
     <row r="34" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H34" s="4"/>
     </row>
     <row r="35" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D35" s="6">
         <v>7</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H35" s="4"/>
     </row>
     <row r="36" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D36" s="6">
         <v>7</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H36" s="4"/>
     </row>
     <row r="37" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H37" s="4"/>
     </row>
     <row r="38" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D38" s="6">
         <v>4</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H38" s="4"/>
     </row>
     <row r="39" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D39" s="6">
         <v>7</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H39" s="4"/>
     </row>
     <row r="40" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D40" s="6">
         <v>7</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H40" s="4"/>
     </row>
     <row r="41" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D41" s="6">
         <v>4</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H41" s="4"/>
     </row>
     <row r="42" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D42" s="6">
         <v>4</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H42" s="4"/>
     </row>
     <row r="43" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D43" s="6">
         <v>4</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H43" s="4"/>
     </row>
     <row r="44" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D44" s="6">
         <v>7</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H44" s="4"/>
     </row>
     <row r="45" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D45" s="6">
         <v>4</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H45" s="4"/>
     </row>
     <row r="46" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H46" s="4"/>
     </row>
     <row r="47" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H47" s="4"/>
     </row>
     <row r="48" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H48" s="4"/>
     </row>
     <row r="49" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H49" s="4"/>
     </row>
     <row r="50" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H50" s="4"/>
     </row>
     <row r="51" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H51" s="4"/>
     </row>
     <row r="52" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H52" s="4"/>
     </row>
     <row r="53" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H53" s="4"/>
     </row>
     <row r="54" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H54" s="4"/>
     </row>
     <row r="55" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="H55" s="4"/>
     </row>
     <row r="56" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H56" s="4"/>
     </row>
     <row r="57" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H57" s="4"/>
     </row>
     <row r="58" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H58" s="4"/>
     </row>
     <row r="59" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H59" s="4"/>
     </row>
     <row r="60" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="H60" s="4"/>
     </row>
     <row r="61" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="H61" s="4"/>
     </row>
     <row r="62" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H62" s="4"/>
     </row>
     <row r="63" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>109</v>
+        <v>49</v>
       </c>
       <c r="D63" s="12">
         <v>4</v>
       </c>
       <c r="E63" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H63" s="4"/>
     </row>
     <row r="64" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D64" s="12">
         <v>4</v>
       </c>
       <c r="E64" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H64" s="4"/>
     </row>
     <row r="65" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="12" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D65" s="12">
         <v>4</v>
       </c>
       <c r="E65" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H65" s="4"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D67" s="4">
         <v>3</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="D69" s="4">
         <v>1</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B70" s="10" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="D70" s="4">
         <v>9</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="D71" s="4">
         <v>10</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="D72" s="4">
         <v>9</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -3067,21 +3060,21 @@
   <sheetData>
     <row r="1" spans="1:3" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="B2" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -3089,10 +3082,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B3" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -3100,10 +3093,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B4" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -3111,10 +3104,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -3122,10 +3115,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="B6" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -3133,10 +3126,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -3144,10 +3137,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -3155,10 +3148,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -3166,10 +3159,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B10" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -3177,10 +3170,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="B11" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -3211,121 +3204,121 @@
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
         <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B9" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F10" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B11" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B12" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
         <v>15</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -3337,8 +3330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B15F685-1533-4446-BC92-30DBE05F964F}">
   <dimension ref="A1:F67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:F67"/>
+    <sheetView topLeftCell="A53" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3353,1022 +3346,1022 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
     </row>
     <row r="3" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E3" s="14"/>
       <c r="F3" s="14"/>
     </row>
     <row r="4" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>59</v>
+        <v>285</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
     </row>
     <row r="5" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
     </row>
     <row r="6" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
     </row>
     <row r="8" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
     </row>
     <row r="12" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
     </row>
     <row r="13" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
     </row>
     <row r="14" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
     </row>
     <row r="15" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
     </row>
     <row r="16" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E16" s="14"/>
       <c r="F16" s="14"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E18" s="14"/>
       <c r="F18" s="18"/>
     </row>
     <row r="19" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E19" s="14"/>
       <c r="F19" s="18"/>
     </row>
     <row r="20" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E20" s="14"/>
       <c r="F20" s="18"/>
     </row>
     <row r="21" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E21" s="14"/>
       <c r="F21" s="18"/>
     </row>
     <row r="22" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E22" s="14"/>
       <c r="F22" s="18"/>
     </row>
     <row r="23" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E23" s="14"/>
       <c r="F23" s="18"/>
     </row>
     <row r="24" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E24" s="14"/>
       <c r="F24" s="18"/>
     </row>
     <row r="25" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E25" s="14"/>
       <c r="F25" s="18"/>
     </row>
     <row r="26" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E26" s="14"/>
       <c r="F26" s="18"/>
     </row>
     <row r="27" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E27" s="14"/>
       <c r="F27" s="18"/>
     </row>
     <row r="28" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E28" s="14"/>
       <c r="F28" s="18"/>
     </row>
     <row r="29" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E29" s="14"/>
       <c r="F29" s="18"/>
     </row>
     <row r="30" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E30" s="14"/>
       <c r="F30" s="18"/>
     </row>
     <row r="31" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E31" s="14"/>
       <c r="F31" s="18"/>
     </row>
     <row r="32" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E32" s="14"/>
       <c r="F32" s="18"/>
     </row>
     <row r="33" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E33" s="14"/>
       <c r="F33" s="18"/>
     </row>
     <row r="34" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E34" s="14"/>
       <c r="F34" s="18"/>
     </row>
     <row r="35" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B35" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="18" t="s">
         <v>41</v>
-      </c>
-      <c r="C35" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="D35" s="18" t="s">
-        <v>42</v>
       </c>
       <c r="E35" s="14"/>
       <c r="F35" s="18"/>
     </row>
     <row r="36" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B36" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" s="19" t="s">
         <v>39</v>
-      </c>
-      <c r="C36" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="D36" s="19" t="s">
-        <v>40</v>
       </c>
       <c r="E36" s="14"/>
       <c r="F36" s="18"/>
     </row>
     <row r="37" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>0</v>
+        <v>285</v>
       </c>
       <c r="E37" s="14"/>
       <c r="F37" s="18"/>
     </row>
     <row r="38" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E38" s="14"/>
       <c r="F38" s="18"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B40" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E40" s="14"/>
       <c r="F40" s="22"/>
     </row>
     <row r="41" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="22" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C41" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>59</v>
+        <v>285</v>
       </c>
       <c r="E41" s="14"/>
       <c r="F41" s="22"/>
     </row>
     <row r="42" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="22" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B42" s="23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D42" s="23" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E42" s="14"/>
       <c r="F42" s="22"/>
     </row>
     <row r="43" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B43" s="23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E43" s="14"/>
       <c r="F43" s="22"/>
     </row>
     <row r="44" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B44" s="23" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D44" s="23" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E44" s="14"/>
       <c r="F44" s="22"/>
     </row>
     <row r="45" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B45" s="23" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C45" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D45" s="23" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E45" s="14"/>
       <c r="F45" s="22"/>
     </row>
     <row r="46" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="22" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B46" s="23" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C46" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D46" s="23" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E46" s="14"/>
       <c r="F46" s="22"/>
     </row>
     <row r="47" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B47" s="23" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C47" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D47" s="23" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E47" s="14"/>
       <c r="F47" s="22"/>
     </row>
     <row r="48" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C48" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D48" s="23" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E48" s="14"/>
       <c r="F48" s="22"/>
     </row>
     <row r="49" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="22" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B49" s="23" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C49" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D49" s="23" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E49" s="14"/>
       <c r="F49" s="22"/>
     </row>
     <row r="50" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="22" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B50" s="23" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C50" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D50" s="23" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E50" s="14"/>
       <c r="F50" s="22"/>
     </row>
     <row r="51" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="22" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B51" s="23" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C51" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D51" s="23" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E51" s="14"/>
       <c r="F51" s="22"/>
     </row>
     <row r="52" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="22" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B52" s="23" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C52" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D52" s="23" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E52" s="14"/>
       <c r="F52" s="22"/>
     </row>
     <row r="53" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="22" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B53" s="23" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C53" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D53" s="23" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E53" s="14"/>
       <c r="F53" s="22"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="55" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="28" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B55" s="29" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C55" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D55" s="29" t="s">
-        <v>59</v>
+        <v>285</v>
       </c>
       <c r="E55" s="14"/>
       <c r="F55" s="28"/>
     </row>
     <row r="56" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="28" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B56" s="29" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C56" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D56" s="29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E56" s="14"/>
       <c r="F56" s="28"/>
     </row>
     <row r="57" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="28" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B57" s="29" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C57" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D57" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E57" s="14"/>
       <c r="F57" s="28"/>
     </row>
     <row r="58" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="28" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B58" s="29" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C58" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D58" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E58" s="14"/>
       <c r="F58" s="28"/>
     </row>
     <row r="59" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="28" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B59" s="29" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C59" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D59" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E59" s="14"/>
       <c r="F59" s="28"/>
     </row>
     <row r="60" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="28" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B60" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C60" s="30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D60" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E60" s="14"/>
       <c r="F60" s="28"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D62" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E62" s="14"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E63" s="14"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="E64" s="14"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="E65" s="14"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E66" s="14"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D67" s="10" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="E67" s="14"/>
     </row>
@@ -4393,6 +4386,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="0c85289e-a0a4-4193-8a36-83840327cccf" xsi:nil="true"/>
@@ -4401,15 +4403,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4668,6 +4661,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4B4AC16-F988-4D41-8F01-205FCE01B916}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{084C8915-1C39-4800-8751-2F69F55F51E7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -4680,14 +4681,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="0c85289e-a0a4-4193-8a36-83840327cccf"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4B4AC16-F988-4D41-8F01-205FCE01B916}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
updating with Maryanne's edits
</commit_message>
<xml_diff>
--- a/EMFOConceptsAndRelationships.xlsx
+++ b/EMFOConceptsAndRelationships.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\softwareRepos\EcologicalMentalFunctioningOntology\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guydi\work\softwareRepos\EcologicalMentalFunctioningOntology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6187FF8-A250-41D9-A3C3-434C7A958046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA366656-F4A9-40ED-9733-AC54E3EC4A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="3420" windowWidth="23100" windowHeight="11700" tabRatio="946" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="946" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="293">
   <si>
     <t>Output</t>
   </si>
@@ -96,9 +96,6 @@
     <t>integrates</t>
   </si>
   <si>
-    <t>is necessary for</t>
-  </si>
-  <si>
     <t>uses</t>
   </si>
   <si>
@@ -453,9 +450,6 @@
     <t>EMFO_C005547</t>
   </si>
   <si>
-    <t>EMFO_C022668</t>
-  </si>
-  <si>
     <t>EMFO_C017617</t>
   </si>
   <si>
@@ -895,6 +889,33 @@
   </si>
   <si>
     <t>Ecological_Mental_Functioning_Ontology</t>
+  </si>
+  <si>
+    <t>Impairments</t>
+  </si>
+  <si>
+    <t>NEEDS_ID</t>
+  </si>
+  <si>
+    <t>Mental_Activity_Limitations</t>
+  </si>
+  <si>
+    <t>Some Definition</t>
+  </si>
+  <si>
+    <t>Geneneral_Tasks_and_Demands</t>
+  </si>
+  <si>
+    <t>(some)_have</t>
+  </si>
+  <si>
+    <t>EMFO_R00010</t>
+  </si>
+  <si>
+    <t>NEEDS_RS_ID</t>
+  </si>
+  <si>
+    <t>has</t>
   </si>
 </sst>
 </file>
@@ -1581,11 +1602,11 @@
   </tableStyles>
   <colors>
     <mruColors>
-      <color rgb="FFFFCFB7"/>
       <color rgb="FFF0D9FF"/>
-      <color rgb="FFCE85FF"/>
       <color rgb="FFFFD6C1"/>
       <color rgb="FFFFCC99"/>
+      <color rgb="FFFFCFB7"/>
+      <color rgb="FFCE85FF"/>
       <color rgb="FFD9F0C8"/>
     </mruColors>
   </colors>
@@ -1897,10 +1918,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H72"/>
+  <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1927,13 +1948,13 @@
         <v>10</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>5</v>
@@ -1941,13 +1962,13 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2" s="4">
         <v>6</v>
@@ -1959,69 +1980,69 @@
         <v>7</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" s="4">
         <v>1</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="D6" s="4">
         <v>4</v>
@@ -2032,13 +2053,13 @@
     </row>
     <row r="7" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="5">
         <v>4</v>
@@ -2050,19 +2071,19 @@
         <v>8</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="5">
         <v>8</v>
@@ -2074,19 +2095,19 @@
         <v>6</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>116</v>
+        <v>285</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>62</v>
+        <v>286</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="5">
         <v>7</v>
@@ -2098,124 +2119,124 @@
         <v>9</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>63</v>
+        <v>287</v>
       </c>
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+      <c r="D10" s="5">
+        <v>7</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>62</v>
       </c>
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="5">
-        <v>7</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="C12" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5">
+        <v>7</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="D12" s="5">
-        <v>7</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>65</v>
       </c>
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>66</v>
+        <v>4</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="D13" s="5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D14" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>4</v>
@@ -2230,16 +2251,16 @@
         <v>9</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>4</v>
@@ -2254,16 +2275,16 @@
         <v>9</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>4</v>
@@ -2278,16 +2299,16 @@
         <v>9</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>4</v>
@@ -2302,16 +2323,16 @@
         <v>9</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H18" s="4"/>
     </row>
     <row r="19" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>4</v>
@@ -2326,16 +2347,16 @@
         <v>9</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H19" s="4"/>
     </row>
     <row r="20" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>4</v>
@@ -2350,16 +2371,16 @@
         <v>9</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H20" s="4"/>
     </row>
     <row r="21" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>4</v>
@@ -2374,301 +2395,466 @@
         <v>9</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H21" s="4"/>
     </row>
     <row r="22" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="5">
+        <v>7</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="H22" s="4"/>
     </row>
     <row r="23" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>284</v>
+        <v>128</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="5">
+        <v>7</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="H23" s="4"/>
     </row>
     <row r="24" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>76</v>
+        <v>129</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="D24" s="5">
+        <v>7</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="H24" s="4"/>
     </row>
     <row r="25" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="D25" s="5">
+        <v>7</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="H25" s="4"/>
     </row>
     <row r="26" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>283</v>
+        <v>131</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="D26" s="5">
+        <v>7</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="H26" s="4"/>
     </row>
-    <row r="27" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D27" s="6">
-        <v>7</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>9</v>
+    <row r="27" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="D27" s="5">
+        <v>7</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="H27" s="4"/>
     </row>
     <row r="28" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>36</v>
+        <v>23</v>
+      </c>
+      <c r="D28" s="6">
+        <v>7</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>287</v>
       </c>
       <c r="H28" s="4"/>
     </row>
     <row r="29" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D29" s="6">
-        <v>7</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>9</v>
+        <v>35</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>287</v>
       </c>
       <c r="H29" s="4"/>
     </row>
     <row r="30" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>137</v>
+        <v>285</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>80</v>
+        <v>284</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="D30" s="6">
+        <v>7</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>287</v>
       </c>
       <c r="H30" s="4"/>
     </row>
     <row r="31" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
+      </c>
+      <c r="D31" s="6">
+        <v>7</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>287</v>
       </c>
       <c r="H31" s="4"/>
     </row>
     <row r="32" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>78</v>
+        <v>23</v>
+      </c>
+      <c r="D32" s="6">
+        <v>7</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>287</v>
       </c>
       <c r="H32" s="4"/>
     </row>
     <row r="33" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D33" s="6">
-        <v>4</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>8</v>
+        <v>80</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>287</v>
       </c>
       <c r="H33" s="4"/>
     </row>
     <row r="34" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>81</v>
+        <v>39</v>
+      </c>
+      <c r="D34" s="6">
+        <v>4</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>287</v>
       </c>
       <c r="H34" s="4"/>
     </row>
     <row r="35" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>82</v>
+        <v>40</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D35" s="6">
-        <v>7</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>9</v>
+        <v>80</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>287</v>
       </c>
       <c r="H35" s="4"/>
     </row>
     <row r="36" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D36" s="6">
         <v>7</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>9</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>287</v>
       </c>
       <c r="H36" s="4"/>
     </row>
     <row r="37" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>85</v>
+        <v>79</v>
+      </c>
+      <c r="D37" s="6">
+        <v>7</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>287</v>
       </c>
       <c r="H37" s="4"/>
     </row>
     <row r="38" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>84</v>
       </c>
       <c r="D38" s="6">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>287</v>
       </c>
       <c r="H38" s="4"/>
     </row>
     <row r="39" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D39" s="6">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>287</v>
       </c>
       <c r="H39" s="4"/>
     </row>
     <row r="40" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D40" s="6">
         <v>7</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>9</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>287</v>
       </c>
       <c r="H40" s="4"/>
     </row>
     <row r="41" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D41" s="6">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>287</v>
       </c>
       <c r="H41" s="4"/>
     </row>
     <row r="42" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D42" s="6">
         <v>4</v>
@@ -2676,17 +2862,23 @@
       <c r="E42" s="6" t="s">
         <v>8</v>
       </c>
+      <c r="F42" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>287</v>
+      </c>
       <c r="H42" s="4"/>
     </row>
     <row r="43" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D43" s="6">
         <v>4</v>
@@ -2694,227 +2886,497 @@
       <c r="E43" s="6" t="s">
         <v>8</v>
       </c>
+      <c r="F43" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>287</v>
+      </c>
       <c r="H43" s="4"/>
     </row>
     <row r="44" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>44</v>
+        <v>89</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="D44" s="6">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>287</v>
       </c>
       <c r="H44" s="4"/>
     </row>
     <row r="45" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D45" s="6">
+        <v>7</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D46" s="6">
         <v>4</v>
       </c>
-      <c r="E45" s="6" t="s">
+      <c r="E46" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H45" s="4"/>
-    </row>
-    <row r="46" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>27</v>
+      <c r="F46" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>287</v>
       </c>
       <c r="H46" s="4"/>
     </row>
     <row r="47" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>91</v>
+        <v>45</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>46</v>
+        <v>26</v>
+      </c>
+      <c r="D47" s="7">
+        <v>4</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>287</v>
       </c>
       <c r="H47" s="4"/>
     </row>
     <row r="48" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>47</v>
+        <v>90</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>91</v>
+        <v>25</v>
+      </c>
+      <c r="D48" s="7">
+        <v>4</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>287</v>
       </c>
       <c r="H48" s="4"/>
     </row>
     <row r="49" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
+      </c>
+      <c r="D49" s="7">
+        <v>4</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>287</v>
       </c>
       <c r="H49" s="4"/>
     </row>
     <row r="50" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>92</v>
+        <v>47</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D50" s="7">
+        <v>4</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>287</v>
       </c>
       <c r="H50" s="4"/>
     </row>
     <row r="51" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>92</v>
+        <v>25</v>
+      </c>
+      <c r="D51" s="7">
+        <v>4</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>287</v>
       </c>
       <c r="H51" s="4"/>
     </row>
     <row r="52" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D52" s="7">
+        <v>4</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>287</v>
       </c>
       <c r="H52" s="4"/>
     </row>
     <row r="53" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D53" s="7">
+        <v>4</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>287</v>
       </c>
       <c r="H53" s="4"/>
     </row>
     <row r="54" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D54" s="7">
+        <v>4</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G54" s="7" t="s">
+        <v>287</v>
       </c>
       <c r="H54" s="4"/>
     </row>
     <row r="55" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D55" s="7">
+        <v>4</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>287</v>
       </c>
       <c r="H55" s="4"/>
     </row>
     <row r="56" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D56" s="7">
+        <v>4</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>287</v>
       </c>
       <c r="H56" s="4"/>
     </row>
     <row r="57" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D57" s="7">
+        <v>4</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>287</v>
       </c>
       <c r="H57" s="4"/>
     </row>
     <row r="58" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D58" s="7">
+        <v>4</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G58" s="7" t="s">
+        <v>287</v>
       </c>
       <c r="H58" s="4"/>
     </row>
     <row r="59" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D59" s="7">
+        <v>4</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>287</v>
       </c>
       <c r="H59" s="4"/>
     </row>
     <row r="60" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D60" s="7">
+        <v>4</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G60" s="7" t="s">
+        <v>287</v>
       </c>
       <c r="H60" s="4"/>
     </row>
     <row r="61" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D61" s="7">
+        <v>4</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G61" s="7" t="s">
+        <v>287</v>
       </c>
       <c r="H61" s="4"/>
     </row>
     <row r="62" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D62" s="7">
+        <v>4</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G62" s="7" t="s">
+        <v>287</v>
       </c>
       <c r="H62" s="4"/>
     </row>
-    <row r="63" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="B63" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D63" s="12">
+    <row r="63" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D63" s="7">
         <v>4</v>
       </c>
-      <c r="E63" s="12" t="s">
+      <c r="E63" s="7" t="s">
         <v>8</v>
+      </c>
+      <c r="F63" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G63" s="7" t="s">
+        <v>287</v>
       </c>
       <c r="H63" s="4"/>
     </row>
     <row r="64" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>106</v>
+        <v>48</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="D64" s="12">
         <v>4</v>
@@ -2922,14 +3384,23 @@
       <c r="E64" s="12" t="s">
         <v>8</v>
       </c>
+      <c r="F64" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G64" s="12" t="s">
+        <v>287</v>
+      </c>
       <c r="H64" s="4"/>
     </row>
     <row r="65" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="12" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>107</v>
+        <v>105</v>
+      </c>
+      <c r="C65" s="12" t="s">
+        <v>48</v>
       </c>
       <c r="D65" s="12">
         <v>4</v>
@@ -2937,105 +3408,135 @@
       <c r="E65" s="12" t="s">
         <v>8</v>
       </c>
+      <c r="F65" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G65" s="12" t="s">
+        <v>287</v>
+      </c>
       <c r="H65" s="4"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="D67" s="4">
-        <v>3</v>
-      </c>
-      <c r="E67" s="4" t="s">
-        <v>248</v>
-      </c>
+    <row r="66" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B66" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C66" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D66" s="12">
+        <v>4</v>
+      </c>
+      <c r="E66" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F66" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G66" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="H66" s="4"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>261</v>
+        <v>242</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>282</v>
+        <v>241</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>262</v>
+        <v>258</v>
+      </c>
+      <c r="D68" s="4">
+        <v>3</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>262</v>
+        <v>280</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="D69" s="4">
-        <v>1</v>
+        <v>260</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="B70" s="10" t="s">
-        <v>265</v>
+        <v>261</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>260</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>262</v>
       </c>
       <c r="D70" s="4">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>23</v>
+        <v>263</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="D71" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>266</v>
+        <v>22</v>
       </c>
       <c r="C72" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="D72" s="4">
+        <v>10</v>
+      </c>
+      <c r="E72" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="D72" s="4">
-        <v>9</v>
-      </c>
-      <c r="E72" s="4" t="s">
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="B73" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="C73" s="4" t="s">
         <v>267</v>
+      </c>
+      <c r="D73" s="4">
+        <v>9</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -3060,21 +3561,21 @@
   <sheetData>
     <row r="1" spans="1:3" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -3082,10 +3583,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -3093,10 +3594,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -3104,7 +3605,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -3115,10 +3616,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B6" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -3126,7 +3627,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -3137,7 +3638,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -3151,7 +3652,7 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -3159,10 +3660,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B10" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -3170,10 +3671,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B11" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -3186,10 +3687,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D798B18-C5BD-476F-9FF2-CDB45434B078}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3204,22 +3705,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3235,7 +3736,7 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3243,7 +3744,7 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3251,66 +3752,66 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B9" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B12" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -3319,6 +3820,14 @@
       </c>
       <c r="B13" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>289</v>
+      </c>
+      <c r="B14" t="s">
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -3328,10 +3837,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B15F685-1533-4446-BC92-30DBE05F964F}">
-  <dimension ref="A1:F67"/>
+  <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3346,257 +3855,257 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
     </row>
     <row r="3" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" s="14"/>
       <c r="F3" s="14"/>
     </row>
     <row r="4" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
     </row>
     <row r="5" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
     </row>
     <row r="6" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
     </row>
     <row r="8" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
     </row>
     <row r="12" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
     </row>
     <row r="13" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
     </row>
     <row r="14" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
     </row>
     <row r="15" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
     </row>
     <row r="16" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>1</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>3</v>
@@ -3604,766 +4113,878 @@
       <c r="E16" s="14"/>
       <c r="F16" s="14"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
-        <v>201</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>33</v>
+    <row r="17" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>286</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>289</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+    </row>
+    <row r="18" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>19</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="E18" s="14"/>
-      <c r="F18" s="18"/>
-    </row>
-    <row r="19" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
-        <v>202</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>78</v>
+      <c r="F18" s="14"/>
+    </row>
+    <row r="19" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>48</v>
       </c>
       <c r="E19" s="14"/>
-      <c r="F19" s="18"/>
-    </row>
-    <row r="20" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
-        <v>203</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>33</v>
+      <c r="F19" s="14"/>
+    </row>
+    <row r="20" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>19</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="E20" s="14"/>
-      <c r="F20" s="18"/>
-    </row>
-    <row r="21" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
-        <v>204</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="E21" s="14"/>
-      <c r="F21" s="18"/>
+      <c r="F20" s="14"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="22" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>82</v>
+        <v>35</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>78</v>
+        <v>24</v>
       </c>
       <c r="E22" s="14"/>
       <c r="F22" s="18"/>
     </row>
     <row r="23" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E23" s="14"/>
       <c r="F23" s="18"/>
     </row>
     <row r="24" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E24" s="14"/>
       <c r="F24" s="18"/>
     </row>
     <row r="25" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E25" s="14"/>
       <c r="F25" s="18"/>
     </row>
     <row r="26" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
-        <v>209</v>
+        <v>291</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>33</v>
+        <v>289</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>85</v>
+        <v>284</v>
       </c>
       <c r="E26" s="14"/>
       <c r="F26" s="18"/>
     </row>
     <row r="27" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
-        <v>210</v>
+        <v>291</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>33</v>
+        <v>289</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>80</v>
+        <v>284</v>
       </c>
       <c r="E27" s="14"/>
       <c r="F27" s="18"/>
     </row>
     <row r="28" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E28" s="14"/>
       <c r="F28" s="18"/>
     </row>
     <row r="29" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E29" s="14"/>
       <c r="F29" s="18"/>
     </row>
     <row r="30" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E30" s="14"/>
       <c r="F30" s="18"/>
     </row>
     <row r="31" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>45</v>
+        <v>83</v>
       </c>
       <c r="E31" s="14"/>
       <c r="F31" s="18"/>
     </row>
     <row r="32" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
-        <v>215</v>
-      </c>
-      <c r="B32" s="18" t="s">
-        <v>40</v>
+        <v>207</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>86</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="D32" s="18" t="s">
-        <v>43</v>
+        <v>32</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>83</v>
       </c>
       <c r="E32" s="14"/>
       <c r="F32" s="18"/>
     </row>
     <row r="33" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
       <c r="E33" s="14"/>
       <c r="F33" s="18"/>
     </row>
     <row r="34" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="C34" s="18" t="s">
-        <v>18</v>
+        <v>87</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>32</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="E34" s="14"/>
       <c r="F34" s="18"/>
     </row>
     <row r="35" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
-        <v>218</v>
-      </c>
-      <c r="B35" s="18" t="s">
-        <v>40</v>
+        <v>210</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>88</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="D35" s="18" t="s">
-        <v>41</v>
+        <v>32</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>81</v>
       </c>
       <c r="E35" s="14"/>
       <c r="F35" s="18"/>
     </row>
     <row r="36" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C36" s="26" t="s">
-        <v>50</v>
+        <v>89</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>32</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="E36" s="14"/>
       <c r="F36" s="18"/>
     </row>
     <row r="37" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="B37" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C37" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>285</v>
+        <v>212</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>44</v>
       </c>
       <c r="E37" s="14"/>
       <c r="F37" s="18"/>
     </row>
     <row r="38" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="B38" s="19" t="s">
+        <v>213</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38" s="18" t="s">
         <v>42</v>
-      </c>
-      <c r="C38" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D38" s="19" t="s">
-        <v>44</v>
       </c>
       <c r="E38" s="14"/>
       <c r="F38" s="18"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="22" t="s">
-        <v>222</v>
-      </c>
-      <c r="B40" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C40" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="D40" s="23" t="s">
-        <v>27</v>
+    <row r="39" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E39" s="14"/>
+      <c r="F39" s="18"/>
+    </row>
+    <row r="40" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>36</v>
       </c>
       <c r="E40" s="14"/>
-      <c r="F40" s="22"/>
-    </row>
-    <row r="41" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="22" t="s">
-        <v>223</v>
-      </c>
-      <c r="B41" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C41" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="D41" s="23" t="s">
-        <v>285</v>
+      <c r="F40" s="18"/>
+    </row>
+    <row r="41" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="18" t="s">
+        <v>216</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>40</v>
       </c>
       <c r="E41" s="14"/>
-      <c r="F41" s="22"/>
-    </row>
-    <row r="42" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="22" t="s">
-        <v>224</v>
-      </c>
-      <c r="B42" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="C42" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="D42" s="23" t="s">
-        <v>91</v>
+      <c r="F41" s="18"/>
+    </row>
+    <row r="42" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>38</v>
       </c>
       <c r="E42" s="14"/>
-      <c r="F42" s="22"/>
-    </row>
-    <row r="43" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="22" t="s">
-        <v>225</v>
-      </c>
-      <c r="B43" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="C43" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="D43" s="23" t="s">
-        <v>91</v>
+      <c r="F42" s="18"/>
+    </row>
+    <row r="43" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="B43" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>292</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>77</v>
       </c>
       <c r="E43" s="14"/>
-      <c r="F43" s="22"/>
-    </row>
-    <row r="44" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="22" t="s">
-        <v>226</v>
-      </c>
-      <c r="B44" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="C44" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="D44" s="23" t="s">
-        <v>93</v>
+      <c r="F43" s="18"/>
+    </row>
+    <row r="44" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="B44" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C44" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" s="19" t="s">
+        <v>43</v>
       </c>
       <c r="E44" s="14"/>
-      <c r="F44" s="22"/>
-    </row>
-    <row r="45" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="22" t="s">
-        <v>227</v>
-      </c>
-      <c r="B45" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="C45" s="24" t="s">
-        <v>33</v>
+      <c r="F44" s="18"/>
+    </row>
+    <row r="45" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="18" t="s">
+        <v>291</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>284</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>289</v>
       </c>
       <c r="D45" s="23" t="s">
-        <v>93</v>
+        <v>286</v>
       </c>
       <c r="E45" s="14"/>
-      <c r="F45" s="22"/>
-    </row>
-    <row r="46" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="22" t="s">
-        <v>228</v>
-      </c>
-      <c r="B46" s="23" t="s">
-        <v>96</v>
-      </c>
-      <c r="C46" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="D46" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="E46" s="14"/>
-      <c r="F46" s="22"/>
+      <c r="F45" s="18"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="47" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="B47" s="23" t="s">
-        <v>97</v>
+        <v>45</v>
       </c>
       <c r="C47" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D47" s="23" t="s">
-        <v>93</v>
+        <v>26</v>
       </c>
       <c r="E47" s="14"/>
       <c r="F47" s="22"/>
     </row>
     <row r="48" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>98</v>
+        <v>45</v>
       </c>
       <c r="C48" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D48" s="23" t="s">
-        <v>92</v>
+        <v>283</v>
       </c>
       <c r="E48" s="14"/>
       <c r="F48" s="22"/>
     </row>
     <row r="49" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="22" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="B49" s="23" t="s">
-        <v>99</v>
+        <v>46</v>
       </c>
       <c r="C49" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D49" s="23" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="E49" s="14"/>
       <c r="F49" s="22"/>
     </row>
     <row r="50" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="22" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="B50" s="23" t="s">
-        <v>100</v>
+        <v>47</v>
       </c>
       <c r="C50" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D50" s="23" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="E50" s="14"/>
       <c r="F50" s="22"/>
     </row>
     <row r="51" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="22" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="B51" s="23" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C51" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D51" s="23" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E51" s="14"/>
       <c r="F51" s="22"/>
     </row>
     <row r="52" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="22" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="B52" s="23" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="C52" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D52" s="23" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="E52" s="14"/>
       <c r="F52" s="22"/>
     </row>
     <row r="53" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="22" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="B53" s="23" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C53" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D53" s="23" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="E53" s="14"/>
       <c r="F53" s="22"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="28" t="s">
+    <row r="54" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="B54" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C54" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D54" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="E54" s="14"/>
+      <c r="F54" s="22"/>
+    </row>
+    <row r="55" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="B55" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="C55" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D55" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="E55" s="14"/>
+      <c r="F55" s="22"/>
+    </row>
+    <row r="56" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="B56" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="C56" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D56" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="E56" s="14"/>
+      <c r="F56" s="22"/>
+    </row>
+    <row r="57" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="B57" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="C57" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D57" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="E57" s="14"/>
+      <c r="F57" s="22"/>
+    </row>
+    <row r="58" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="B58" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="C58" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D58" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="E58" s="14"/>
+      <c r="F58" s="22"/>
+    </row>
+    <row r="59" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="22" t="s">
+        <v>232</v>
+      </c>
+      <c r="B59" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="C59" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D59" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="E59" s="14"/>
+      <c r="F59" s="22"/>
+    </row>
+    <row r="60" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="B60" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="C60" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D60" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="E60" s="14"/>
+      <c r="F60" s="22"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="28" t="s">
+        <v>234</v>
+      </c>
+      <c r="B62" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="C62" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D62" s="29" t="s">
+        <v>283</v>
+      </c>
+      <c r="E62" s="14"/>
+      <c r="F62" s="28"/>
+    </row>
+    <row r="63" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="28" t="s">
+        <v>235</v>
+      </c>
+      <c r="B63" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="C63" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D63" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E63" s="14"/>
+      <c r="F63" s="28"/>
+    </row>
+    <row r="64" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="28" t="s">
         <v>236</v>
       </c>
-      <c r="B55" s="29" t="s">
+      <c r="B64" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="C64" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D64" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E64" s="14"/>
+      <c r="F64" s="28"/>
+    </row>
+    <row r="65" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="B65" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="C55" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="D55" s="29" t="s">
-        <v>285</v>
-      </c>
-      <c r="E55" s="14"/>
-      <c r="F55" s="28"/>
-    </row>
-    <row r="56" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="28" t="s">
-        <v>237</v>
-      </c>
-      <c r="B56" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="C56" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="D56" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="E56" s="14"/>
-      <c r="F56" s="28"/>
-    </row>
-    <row r="57" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="28" t="s">
+      <c r="C65" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D65" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="E65" s="14"/>
+      <c r="F65" s="28"/>
+    </row>
+    <row r="66" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="28" t="s">
         <v>238</v>
       </c>
-      <c r="B57" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="C57" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="D57" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="E57" s="14"/>
-      <c r="F57" s="28"/>
-    </row>
-    <row r="58" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="28" t="s">
+      <c r="B66" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="C66" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D66" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="E66" s="14"/>
+      <c r="F66" s="28"/>
+    </row>
+    <row r="67" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="28" t="s">
         <v>239</v>
       </c>
-      <c r="B58" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="C58" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="D58" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="E58" s="14"/>
-      <c r="F58" s="28"/>
-    </row>
-    <row r="59" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="28" t="s">
+      <c r="B67" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C67" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="D67" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="E67" s="14"/>
+      <c r="F67" s="28"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C69" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="B59" s="29" t="s">
-        <v>107</v>
-      </c>
-      <c r="C59" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="D59" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="E59" s="14"/>
-      <c r="F59" s="28"/>
-    </row>
-    <row r="60" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="28" t="s">
+      <c r="D69" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E69" s="14"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="B70" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C70" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="D70" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="B60" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="C60" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="D60" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="E60" s="14"/>
-      <c r="F60" s="28"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
+      <c r="E70" s="14"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="B62" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C62" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="D62" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E62" s="14"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
+      <c r="B71" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C71" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="E71" s="14"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="B63" s="10" t="s">
+      <c r="B72" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="C63" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="D63" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="E63" s="14"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
+      <c r="C72" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="D72" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="E72" s="14"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="B64" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C64" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="D64" s="10" t="s">
-        <v>275</v>
-      </c>
-      <c r="E64" s="14"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="4" t="s">
+      <c r="B73" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C73" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="D73" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E73" s="14"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="B65" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C65" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="D65" s="10" t="s">
-        <v>265</v>
-      </c>
-      <c r="E65" s="14"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="B66" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C66" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="D66" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E66" s="14"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="B67" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C67" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="D67" s="10" t="s">
-        <v>266</v>
-      </c>
-      <c r="E67" s="14"/>
+      <c r="B74" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C74" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="D74" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="E74" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4386,26 +5007,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="0c85289e-a0a4-4193-8a36-83840327cccf" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="48f24ce9-3fee-408f-adaa-6c70c8fcad88">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DC0853FBA342F1439B1E03C364E3AF64" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b473cb13b29a9ff7b19694f6b2f73718">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="48f24ce9-3fee-408f-adaa-6c70c8fcad88" xmlns:ns3="0c85289e-a0a4-4193-8a36-83840327cccf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6fe4fbd77109f000862c0d72bea26d08" ns2:_="" ns3:_="">
     <xsd:import namespace="48f24ce9-3fee-408f-adaa-6c70c8fcad88"/>
@@ -4660,10 +5261,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="0c85289e-a0a4-4193-8a36-83840327cccf" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="48f24ce9-3fee-408f-adaa-6c70c8fcad88">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4B4AC16-F988-4D41-8F01-205FCE01B916}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B2D7522-5BE8-4523-8499-DB76C3F0C9F9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="48f24ce9-3fee-408f-adaa-6c70c8fcad88"/>
+    <ds:schemaRef ds:uri="0c85289e-a0a4-4193-8a36-83840327cccf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4686,20 +5318,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B2D7522-5BE8-4523-8499-DB76C3F0C9F9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4B4AC16-F988-4D41-8F01-205FCE01B916}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="48f24ce9-3fee-408f-adaa-6c70c8fcad88"/>
-    <ds:schemaRef ds:uri="0c85289e-a0a4-4193-8a36-83840327cccf"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
updated with needed ids
</commit_message>
<xml_diff>
--- a/EMFOConceptsAndRelationships.xlsx
+++ b/EMFOConceptsAndRelationships.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guydi\work\softwareRepos\EcologicalMentalFunctioningOntology\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\divitag2\work\softwareRepos\EcologicalMentalFunctioningOntology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA366656-F4A9-40ED-9733-AC54E3EC4A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8EF4770-F0A1-4AA5-AE43-E7DC43C06821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="946" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="22410" windowHeight="10665" tabRatio="946" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="300">
   <si>
     <t>Output</t>
   </si>
@@ -894,9 +894,6 @@
     <t>Impairments</t>
   </si>
   <si>
-    <t>NEEDS_ID</t>
-  </si>
-  <si>
     <t>Mental_Activity_Limitations</t>
   </si>
   <si>
@@ -912,10 +909,34 @@
     <t>EMFO_R00010</t>
   </si>
   <si>
-    <t>NEEDS_RS_ID</t>
-  </si>
-  <si>
     <t>has</t>
+  </si>
+  <si>
+    <t>EMFO_C688861</t>
+  </si>
+  <si>
+    <t>EMFO_C611497</t>
+  </si>
+  <si>
+    <t>EMFO_RS_603159</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0530221</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0861683</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0797719</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0766961</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0456265</t>
+  </si>
+  <si>
+    <t>EMFO_RS_0975780</t>
   </si>
 </sst>
 </file>
@@ -1622,9 +1643,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1662,7 +1683,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1768,7 +1789,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1910,7 +1931,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1920,8 +1941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2101,10 +2122,10 @@
     </row>
     <row r="9" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>285</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>286</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>26</v>
@@ -2119,7 +2140,7 @@
         <v>9</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H9" s="4"/>
     </row>
@@ -2455,7 +2476,7 @@
         <v>282</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D24" s="5">
         <v>7</v>
@@ -2479,7 +2500,7 @@
         <v>75</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D25" s="5">
         <v>7</v>
@@ -2503,7 +2524,7 @@
         <v>76</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D26" s="5">
         <v>7</v>
@@ -2527,7 +2548,7 @@
         <v>281</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D27" s="5">
         <v>7</v>
@@ -2563,7 +2584,7 @@
         <v>9</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H28" s="4"/>
     </row>
@@ -2578,13 +2599,13 @@
         <v>35</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H29" s="4"/>
     </row>
     <row r="30" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>285</v>
+        <v>292</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>284</v>
@@ -2602,7 +2623,7 @@
         <v>9</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H30" s="4"/>
     </row>
@@ -2626,7 +2647,7 @@
         <v>9</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H31" s="4"/>
     </row>
@@ -2650,7 +2671,7 @@
         <v>9</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H32" s="4"/>
     </row>
@@ -2665,7 +2686,7 @@
         <v>77</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H33" s="4"/>
     </row>
@@ -2683,7 +2704,7 @@
         <v>8</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H34" s="4"/>
     </row>
@@ -2698,7 +2719,7 @@
         <v>80</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H35" s="4"/>
     </row>
@@ -2722,7 +2743,7 @@
         <v>9</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H36" s="4"/>
     </row>
@@ -2746,7 +2767,7 @@
         <v>9</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H37" s="4"/>
     </row>
@@ -2770,7 +2791,7 @@
         <v>9</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H38" s="4"/>
     </row>
@@ -2794,7 +2815,7 @@
         <v>7</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H39" s="4"/>
     </row>
@@ -2818,7 +2839,7 @@
         <v>9</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H40" s="4"/>
     </row>
@@ -2842,7 +2863,7 @@
         <v>9</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H41" s="4"/>
     </row>
@@ -2866,7 +2887,7 @@
         <v>7</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H42" s="4"/>
     </row>
@@ -2890,7 +2911,7 @@
         <v>7</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H43" s="4"/>
     </row>
@@ -2914,7 +2935,7 @@
         <v>7</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H44" s="4"/>
     </row>
@@ -2935,7 +2956,7 @@
         <v>9</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H45" s="4"/>
     </row>
@@ -2956,7 +2977,7 @@
         <v>7</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H46" s="4"/>
     </row>
@@ -2980,7 +3001,7 @@
         <v>7</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H47" s="4"/>
     </row>
@@ -3004,7 +3025,7 @@
         <v>7</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H48" s="4"/>
     </row>
@@ -3028,7 +3049,7 @@
         <v>7</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H49" s="4"/>
     </row>
@@ -3052,7 +3073,7 @@
         <v>7</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H50" s="4"/>
     </row>
@@ -3076,7 +3097,7 @@
         <v>7</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H51" s="4"/>
     </row>
@@ -3100,7 +3121,7 @@
         <v>7</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H52" s="4"/>
     </row>
@@ -3124,7 +3145,7 @@
         <v>7</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H53" s="4"/>
     </row>
@@ -3148,7 +3169,7 @@
         <v>7</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H54" s="4"/>
     </row>
@@ -3172,7 +3193,7 @@
         <v>7</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H55" s="4"/>
     </row>
@@ -3196,7 +3217,7 @@
         <v>7</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H56" s="4"/>
     </row>
@@ -3220,7 +3241,7 @@
         <v>7</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H57" s="4"/>
     </row>
@@ -3244,7 +3265,7 @@
         <v>7</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H58" s="4"/>
     </row>
@@ -3268,7 +3289,7 @@
         <v>7</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H59" s="4"/>
     </row>
@@ -3292,7 +3313,7 @@
         <v>7</v>
       </c>
       <c r="G60" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H60" s="4"/>
     </row>
@@ -3316,7 +3337,7 @@
         <v>7</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H61" s="4"/>
     </row>
@@ -3340,7 +3361,7 @@
         <v>7</v>
       </c>
       <c r="G62" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H62" s="4"/>
     </row>
@@ -3364,7 +3385,7 @@
         <v>7</v>
       </c>
       <c r="G63" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H63" s="4"/>
     </row>
@@ -3388,7 +3409,7 @@
         <v>7</v>
       </c>
       <c r="G64" s="12" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H64" s="4"/>
     </row>
@@ -3412,7 +3433,7 @@
         <v>7</v>
       </c>
       <c r="G65" s="12" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H65" s="4"/>
     </row>
@@ -3436,7 +3457,7 @@
         <v>7</v>
       </c>
       <c r="G66" s="12" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H66" s="4"/>
     </row>
@@ -3824,10 +3845,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>288</v>
+      </c>
+      <c r="B14" t="s">
         <v>289</v>
-      </c>
-      <c r="B14" t="s">
-        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -3839,8 +3860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B15F685-1533-4446-BC92-30DBE05F964F}">
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4115,13 +4136,13 @@
     </row>
     <row r="17" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>3</v>
@@ -4131,7 +4152,7 @@
     </row>
     <row r="18" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>59</v>
@@ -4147,7 +4168,7 @@
     </row>
     <row r="19" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>0</v>
@@ -4163,7 +4184,7 @@
     </row>
     <row r="20" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="B20" s="15" t="s">
         <v>0</v>
@@ -4248,13 +4269,13 @@
     </row>
     <row r="26" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="B26" s="19" t="s">
         <v>80</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D26" s="19" t="s">
         <v>284</v>
@@ -4264,13 +4285,13 @@
     </row>
     <row r="27" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B27" s="19" t="s">
         <v>79</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D27" s="19" t="s">
         <v>284</v>
@@ -4526,7 +4547,7 @@
         <v>44</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D43" s="18" t="s">
         <v>77</v>
@@ -4552,16 +4573,16 @@
     </row>
     <row r="45" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="18" t="s">
-        <v>291</v>
+        <v>299</v>
       </c>
       <c r="B45" s="19" t="s">
         <v>284</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D45" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E45" s="14"/>
       <c r="F45" s="18"/>
@@ -5007,6 +5028,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="0c85289e-a0a4-4193-8a36-83840327cccf" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="48f24ce9-3fee-408f-adaa-6c70c8fcad88">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DC0853FBA342F1439B1E03C364E3AF64" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b473cb13b29a9ff7b19694f6b2f73718">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="48f24ce9-3fee-408f-adaa-6c70c8fcad88" xmlns:ns3="0c85289e-a0a4-4193-8a36-83840327cccf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6fe4fbd77109f000862c0d72bea26d08" ns2:_="" ns3:_="">
     <xsd:import namespace="48f24ce9-3fee-408f-adaa-6c70c8fcad88"/>
@@ -5261,17 +5293,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="0c85289e-a0a4-4193-8a36-83840327cccf" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="48f24ce9-3fee-408f-adaa-6c70c8fcad88">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5282,6 +5303,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{084C8915-1C39-4800-8751-2F69F55F51E7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="48f24ce9-3fee-408f-adaa-6c70c8fcad88"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="0c85289e-a0a4-4193-8a36-83840327cccf"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B2D7522-5BE8-4523-8499-DB76C3F0C9F9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5300,23 +5338,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{084C8915-1C39-4800-8751-2F69F55F51E7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="48f24ce9-3fee-408f-adaa-6c70c8fcad88"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="0c85289e-a0a4-4193-8a36-83840327cccf"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4B4AC16-F988-4D41-8F01-205FCE01B916}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
added a definitions sheet to the spreadsheet
</commit_message>
<xml_diff>
--- a/EMFOConceptsAndRelationships.xlsx
+++ b/EMFOConceptsAndRelationships.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\divitag2\work\softwareRepos\EcologicalMentalFunctioningOntology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98756C4-5318-4BF7-9E5D-EECDFE2E99C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E86090-263C-4C85-9037-B412C617897B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35190" yWindow="1455" windowWidth="25785" windowHeight="10560" tabRatio="666" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38265" yWindow="1065" windowWidth="24000" windowHeight="10560" tabRatio="666" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,9 @@
     <sheet name="Relationships" sheetId="2" r:id="rId5"/>
     <sheet name="Technical Notes" sheetId="14" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">classes!$A$1:$H$66</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1168" uniqueCount="411">
   <si>
     <t>Output</t>
   </si>
@@ -923,9 +926,6 @@
   </si>
   <si>
     <t>Ontology ID</t>
-  </si>
-  <si>
-    <t>Ontology Concept Name</t>
   </si>
   <si>
     <t>UMLS Concept Name</t>
@@ -2122,9 +2122,6 @@
     <t>not seen in clinical usage</t>
   </si>
   <si>
-    <t>Definition Needed4</t>
-  </si>
-  <si>
     <t>Tree/Quadrant</t>
   </si>
   <si>
@@ -2138,6 +2135,12 @@
   </si>
   <si>
     <t>Throughput/Input</t>
+  </si>
+  <si>
+    <t>Subclass</t>
+  </si>
+  <si>
+    <t>Ontology Class Name</t>
   </si>
 </sst>
 </file>
@@ -2852,7 +2855,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2941,6 +2944,8 @@
     <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="41" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3308,10 +3313,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3350,7 +3356,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -3376,7 +3382,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="45" t="s">
         <v>28</v>
       </c>
@@ -3398,7 +3404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>29</v>
       </c>
@@ -3420,7 +3426,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>30</v>
       </c>
@@ -3442,7 +3448,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>138</v>
       </c>
@@ -3464,7 +3470,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>139</v>
       </c>
@@ -3493,7 +3499,7 @@
       <c r="J7" s="44"/>
       <c r="K7" s="44"/>
     </row>
-    <row r="8" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>108</v>
       </c>
@@ -3571,7 +3577,7 @@
         <v>9</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>405</v>
+        <v>293</v>
       </c>
       <c r="H10" s="45" t="s">
         <v>0</v>
@@ -3580,7 +3586,7 @@
       <c r="J10" s="44"/>
       <c r="K10" s="44"/>
     </row>
-    <row r="11" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>110</v>
       </c>
@@ -3629,7 +3635,7 @@
       <c r="J12" s="44"/>
       <c r="K12" s="44"/>
     </row>
-    <row r="13" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>112</v>
       </c>
@@ -4064,7 +4070,7 @@
       <c r="J27" s="44"/>
       <c r="K27" s="44"/>
     </row>
-    <row r="28" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>127</v>
       </c>
@@ -4093,7 +4099,7 @@
       <c r="J28" s="44"/>
       <c r="K28" s="44"/>
     </row>
-    <row r="29" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>128</v>
       </c>
@@ -4171,7 +4177,7 @@
       <c r="J31" s="44"/>
       <c r="K31" s="44"/>
     </row>
-    <row r="32" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>130</v>
       </c>
@@ -4200,7 +4206,7 @@
       <c r="J32" s="44"/>
       <c r="K32" s="44"/>
     </row>
-    <row r="33" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>131</v>
       </c>
@@ -4220,7 +4226,7 @@
       <c r="J33" s="44"/>
       <c r="K33" s="44"/>
     </row>
-    <row r="34" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>132</v>
       </c>
@@ -4243,7 +4249,7 @@
       <c r="J34" s="44"/>
       <c r="K34" s="44"/>
     </row>
-    <row r="35" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>133</v>
       </c>
@@ -4350,7 +4356,7 @@
       <c r="J38" s="44"/>
       <c r="K38" s="44"/>
     </row>
-    <row r="39" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>140</v>
       </c>
@@ -4408,7 +4414,7 @@
       <c r="J40" s="44"/>
       <c r="K40" s="44"/>
     </row>
-    <row r="41" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>142</v>
       </c>
@@ -4524,7 +4530,7 @@
       <c r="J44" s="44"/>
       <c r="K44" s="44"/>
     </row>
-    <row r="45" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>146</v>
       </c>
@@ -4550,7 +4556,7 @@
       <c r="J45" s="44"/>
       <c r="K45" s="44"/>
     </row>
-    <row r="46" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>147</v>
       </c>
@@ -4605,7 +4611,7 @@
       <c r="J47" s="44"/>
       <c r="K47" s="44"/>
     </row>
-    <row r="48" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>149</v>
       </c>
@@ -4692,7 +4698,7 @@
       <c r="J50" s="44"/>
       <c r="K50" s="44"/>
     </row>
-    <row r="51" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>152</v>
       </c>
@@ -4982,7 +4988,7 @@
       <c r="J60" s="44"/>
       <c r="K60" s="44"/>
     </row>
-    <row r="61" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>162</v>
       </c>
@@ -5069,7 +5075,7 @@
       <c r="J63" s="44"/>
       <c r="K63" s="44"/>
     </row>
-    <row r="64" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" s="11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="11" t="s">
         <v>165</v>
       </c>
@@ -5287,541 +5293,566 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H66" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="Definition Needed"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48FA0E8E-9A29-4F8F-859E-3694C358FB60}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.7109375" style="32" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" style="32" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" style="32" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="32" customWidth="1"/>
-    <col min="5" max="5" width="61.7109375" style="32" customWidth="1"/>
-    <col min="6" max="6" width="55.140625" style="32" customWidth="1"/>
-    <col min="7" max="7" width="71.7109375" style="32" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" style="32" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" style="32" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" style="32" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="32" customWidth="1"/>
+    <col min="6" max="6" width="61.7109375" style="32" customWidth="1"/>
+    <col min="7" max="7" width="55.140625" style="32" customWidth="1"/>
+    <col min="8" max="8" width="71.7109375" style="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
         <v>294</v>
       </c>
       <c r="B1" s="30" t="s">
+        <v>410</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>409</v>
+      </c>
+      <c r="D1" s="30" t="s">
         <v>295</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="E1" s="30" t="s">
         <v>296</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="F1" s="30" t="s">
         <v>297</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="G1" s="31" t="s">
         <v>298</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="H1" s="30" t="s">
         <v>299</v>
       </c>
-      <c r="G1" s="30" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="178.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" ht="178.5" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
         <v>112</v>
       </c>
       <c r="B2" s="34" t="s">
+        <v>300</v>
+      </c>
+      <c r="C2" s="34"/>
+      <c r="D2" s="35" t="s">
         <v>301</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="E2" s="34" t="s">
         <v>302</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="F2" s="35" t="s">
         <v>303</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="G2" s="35" t="s">
         <v>304</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="H2" s="35" t="s">
         <v>305</v>
       </c>
-      <c r="G2" s="35" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="191.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" ht="191.25" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
         <v>110</v>
       </c>
       <c r="B3" s="32" t="s">
+        <v>307</v>
+      </c>
+      <c r="D3" s="32" t="s">
         <v>308</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="E3" s="32" t="s">
         <v>309</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="F3" s="33" t="s">
         <v>310</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="G3" s="33" t="s">
         <v>311</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="H3" s="33" t="s">
         <v>312</v>
       </c>
-      <c r="G3" s="33" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="37" t="s">
         <v>110</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>308</v>
-      </c>
-      <c r="C4" s="32" t="s">
+        <v>307</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>313</v>
+      </c>
+      <c r="E4" s="32" t="s">
         <v>314</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="F4" s="36" t="s">
         <v>315</v>
       </c>
-      <c r="E4" s="36" t="s">
-        <v>316</v>
-      </c>
-      <c r="F4" s="36"/>
       <c r="G4" s="36"/>
-    </row>
-    <row r="5" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="H4" s="36"/>
+    </row>
+    <row r="5" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
         <v>130</v>
       </c>
       <c r="B5" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="D5" s="32" t="s">
+        <v>316</v>
+      </c>
+      <c r="E5" s="32" t="s">
         <v>317</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="F5" s="33" t="s">
         <v>318</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="G5" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="H5" s="33" t="s">
         <v>319</v>
       </c>
-      <c r="F5" s="33" t="s">
-        <v>319</v>
-      </c>
-      <c r="G5" s="33" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
         <v>131</v>
       </c>
       <c r="B6" s="32" t="s">
+        <v>320</v>
+      </c>
+      <c r="D6" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="E6" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="F6" s="38" t="s">
         <v>323</v>
       </c>
-      <c r="E6" s="38" t="s">
-        <v>324</v>
-      </c>
-      <c r="F6" s="38"/>
       <c r="G6" s="38"/>
-    </row>
-    <row r="7" spans="1:7" ht="178.5" x14ac:dyDescent="0.25">
+      <c r="H6" s="38"/>
+    </row>
+    <row r="7" spans="1:8" ht="178.5" x14ac:dyDescent="0.25">
       <c r="A7" s="39" t="s">
         <v>131</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>321</v>
-      </c>
-      <c r="C7" s="34" t="s">
+        <v>320</v>
+      </c>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34" t="s">
+        <v>324</v>
+      </c>
+      <c r="E7" s="34" t="s">
         <v>325</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="F7" s="35" t="s">
         <v>326</v>
       </c>
-      <c r="E7" s="35" t="s">
+      <c r="G7" s="35" t="s">
         <v>327</v>
       </c>
-      <c r="F7" s="35" t="s">
+      <c r="H7" s="35" t="s">
         <v>328</v>
       </c>
-      <c r="G7" s="35" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="165.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" ht="165.75" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
         <v>133</v>
       </c>
       <c r="B8" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="34"/>
+      <c r="D8" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="E8" s="34" t="s">
+        <v>329</v>
+      </c>
+      <c r="F8" s="35" t="s">
         <v>330</v>
       </c>
-      <c r="E8" s="35" t="s">
+      <c r="G8" s="35" t="s">
         <v>331</v>
       </c>
-      <c r="F8" s="35" t="s">
+      <c r="H8" s="35" t="s">
         <v>332</v>
       </c>
-      <c r="G8" s="35" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="204" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" ht="204" x14ac:dyDescent="0.25">
       <c r="A9" s="37" t="s">
         <v>152</v>
       </c>
       <c r="B9" s="32" t="s">
+        <v>333</v>
+      </c>
+      <c r="D9" s="33" t="s">
         <v>334</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="E9" s="33" t="s">
         <v>335</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="F9" s="33" t="s">
         <v>336</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="G9" s="33" t="s">
         <v>337</v>
       </c>
-      <c r="F9" s="33" t="s">
+      <c r="H9" s="33" t="s">
         <v>338</v>
       </c>
-      <c r="G9" s="33" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="242.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8" ht="178.5" x14ac:dyDescent="0.25">
       <c r="A10" s="34" t="s">
         <v>162</v>
       </c>
       <c r="B10" s="34" t="s">
+        <v>339</v>
+      </c>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="34" t="s">
         <v>340</v>
       </c>
-      <c r="C10" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="34" t="s">
+      <c r="F10" s="35" t="s">
         <v>341</v>
       </c>
-      <c r="E10" s="35" t="s">
+      <c r="G10" s="35" t="s">
         <v>342</v>
       </c>
-      <c r="F10" s="35" t="s">
+      <c r="H10" s="35" t="s">
         <v>343</v>
       </c>
-      <c r="G10" s="35" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="89.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
         <v>149</v>
       </c>
       <c r="B11" s="34" t="s">
+        <v>344</v>
+      </c>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="40" t="s">
+        <v>340</v>
+      </c>
+      <c r="F11" s="35" t="s">
         <v>345</v>
       </c>
-      <c r="C11" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="40" t="s">
-        <v>341</v>
-      </c>
-      <c r="E11" s="35" t="s">
+      <c r="G11" s="35" t="s">
         <v>346</v>
       </c>
-      <c r="F11" s="35" t="s">
+      <c r="H11" s="35" t="s">
         <v>347</v>
       </c>
-      <c r="G11" s="35" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A12" s="34" t="s">
         <v>165</v>
       </c>
       <c r="B12" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="34"/>
+      <c r="D12" s="35" t="s">
+        <v>348</v>
+      </c>
+      <c r="E12" s="34" t="s">
         <v>349</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="F12" s="35" t="s">
         <v>350</v>
       </c>
-      <c r="E12" s="35" t="s">
+      <c r="G12" s="35" t="s">
         <v>351</v>
       </c>
-      <c r="F12" s="35" t="s">
+      <c r="H12" s="35" t="s">
         <v>352</v>
       </c>
-      <c r="G12" s="35" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A13" s="39" t="s">
         <v>140</v>
       </c>
       <c r="B13" s="34" t="s">
+        <v>353</v>
+      </c>
+      <c r="C13" s="34"/>
+      <c r="D13" s="35" t="s">
         <v>354</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="E13" s="35" t="s">
         <v>355</v>
       </c>
-      <c r="D13" s="35" t="s">
+      <c r="F13" s="35"/>
+      <c r="G13" s="35" t="s">
         <v>356</v>
       </c>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35" t="s">
-        <v>357</v>
-      </c>
-      <c r="G13" s="35"/>
-    </row>
-    <row r="14" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+      <c r="H13" s="35"/>
+    </row>
+    <row r="14" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A14" s="34" t="s">
         <v>148</v>
       </c>
       <c r="B14" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="40" t="s">
+      <c r="C14" s="35"/>
+      <c r="D14" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="40" t="s">
+      <c r="E14" s="40" t="s">
+        <v>357</v>
+      </c>
+      <c r="F14" s="35" t="s">
         <v>358</v>
       </c>
-      <c r="E14" s="35" t="s">
+      <c r="G14" s="34" t="s">
         <v>359</v>
       </c>
-      <c r="F14" s="34" t="s">
+      <c r="H14" s="35" t="s">
         <v>360</v>
       </c>
-      <c r="G14" s="35" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="114.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:8" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A15" s="39" t="s">
         <v>108</v>
       </c>
       <c r="B15" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="34"/>
+      <c r="D15" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="E15" s="34" t="s">
+        <v>361</v>
+      </c>
+      <c r="F15" s="35" t="s">
         <v>362</v>
       </c>
-      <c r="E15" s="35" t="s">
+      <c r="G15" s="35" t="s">
         <v>363</v>
       </c>
-      <c r="F15" s="35" t="s">
+      <c r="H15" s="35" t="s">
         <v>364</v>
       </c>
-      <c r="G15" s="35" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="127.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:8" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
         <v>142</v>
       </c>
       <c r="B16" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="32" t="s">
+      <c r="D16" s="32" t="s">
+        <v>365</v>
+      </c>
+      <c r="E16" s="32" t="s">
         <v>366</v>
       </c>
-      <c r="D16" s="32" t="s">
+      <c r="F16" s="41" t="s">
         <v>367</v>
       </c>
-      <c r="E16" s="41" t="s">
+      <c r="G16" s="33" t="s">
         <v>368</v>
       </c>
-      <c r="F16" s="33" t="s">
+      <c r="H16" s="33" t="s">
         <v>369</v>
       </c>
-      <c r="G16" s="33" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="114.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:8" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A17" s="32" t="s">
         <v>132</v>
       </c>
       <c r="B17" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="32" t="s">
+      <c r="D17" s="32" t="s">
+        <v>370</v>
+      </c>
+      <c r="E17" s="32" t="s">
         <v>371</v>
       </c>
-      <c r="D17" s="32" t="s">
+      <c r="F17" s="33" t="s">
         <v>372</v>
       </c>
-      <c r="E17" s="33" t="s">
+      <c r="G17" s="33" t="s">
         <v>373</v>
       </c>
-      <c r="F17" s="33" t="s">
+      <c r="H17" s="33" t="s">
         <v>374</v>
       </c>
-      <c r="G17" s="33" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A18" s="39"/>
       <c r="B18" s="34" t="s">
+        <v>375</v>
+      </c>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34" t="s">
         <v>376</v>
       </c>
-      <c r="C18" s="34" t="s">
+      <c r="E18" s="34" t="s">
         <v>377</v>
       </c>
-      <c r="D18" s="34" t="s">
+      <c r="F18" s="35" t="s">
         <v>378</v>
       </c>
-      <c r="E18" s="35" t="s">
+      <c r="G18" s="35" t="s">
         <v>379</v>
       </c>
-      <c r="F18" s="35" t="s">
+      <c r="H18" s="35" t="s">
         <v>380</v>
       </c>
-      <c r="G18" s="35" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A19" s="34" t="s">
         <v>139</v>
       </c>
       <c r="B19" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C19" s="34"/>
+      <c r="D19" s="34" t="s">
+        <v>381</v>
+      </c>
+      <c r="E19" s="34" t="s">
         <v>382</v>
       </c>
-      <c r="D19" s="34" t="s">
+      <c r="F19" s="35" t="s">
         <v>383</v>
       </c>
-      <c r="E19" s="35" t="s">
+      <c r="G19" s="35" t="s">
         <v>384</v>
       </c>
-      <c r="F19" s="35" t="s">
+      <c r="H19" s="35" t="s">
         <v>385</v>
       </c>
-      <c r="G19" s="35" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="102" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:8" ht="102" x14ac:dyDescent="0.25">
       <c r="A20" s="32" t="s">
         <v>146</v>
       </c>
       <c r="B20" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="32" t="s">
+      <c r="D20" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="32" t="s">
-        <v>307</v>
-      </c>
-      <c r="E20" s="33" t="s">
+      <c r="E20" s="32" t="s">
+        <v>306</v>
+      </c>
+      <c r="F20" s="33" t="s">
+        <v>386</v>
+      </c>
+      <c r="G20" s="33" t="s">
         <v>387</v>
       </c>
-      <c r="F20" s="33" t="s">
+      <c r="H20" s="33" t="s">
         <v>388</v>
       </c>
-      <c r="G20" s="33" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A21" s="38" t="s">
         <v>147</v>
       </c>
       <c r="B21" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="38" t="s">
+      <c r="C21" s="42"/>
+      <c r="D21" s="38" t="s">
+        <v>389</v>
+      </c>
+      <c r="E21" s="38" t="s">
         <v>390</v>
       </c>
-      <c r="D21" s="38" t="s">
+      <c r="F21" s="42" t="s">
         <v>391</v>
       </c>
-      <c r="E21" s="42" t="s">
+      <c r="G21" s="42" t="s">
         <v>392</v>
       </c>
-      <c r="F21" s="42" t="s">
+      <c r="H21" s="43" t="s">
         <v>393</v>
       </c>
-      <c r="G21" s="43" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="114.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:8" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A22" s="32" t="s">
         <v>128</v>
       </c>
       <c r="B22" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="34" t="s">
+      <c r="C22" s="34"/>
+      <c r="D22" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="34" t="s">
+      <c r="E22" s="34" t="s">
+        <v>394</v>
+      </c>
+      <c r="F22" s="35" t="s">
         <v>395</v>
       </c>
-      <c r="E22" s="35" t="s">
+      <c r="G22" s="35" t="s">
         <v>396</v>
       </c>
-      <c r="F22" s="35" t="s">
+      <c r="H22" s="35" t="s">
         <v>397</v>
       </c>
-      <c r="G22" s="35" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="89.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:8" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A23" s="39" t="s">
         <v>128</v>
       </c>
       <c r="B23" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="34"/>
+      <c r="D23" s="35" t="s">
+        <v>398</v>
+      </c>
+      <c r="E23" s="35" t="s">
         <v>399</v>
       </c>
-      <c r="D23" s="35" t="s">
+      <c r="F23" s="35" t="s">
         <v>400</v>
       </c>
-      <c r="E23" s="35" t="s">
-        <v>401</v>
-      </c>
-      <c r="F23" s="35"/>
       <c r="G23" s="35"/>
-    </row>
-    <row r="24" spans="1:7" ht="140.25" x14ac:dyDescent="0.25">
+      <c r="H23" s="35"/>
+    </row>
+    <row r="24" spans="1:8" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A24" s="39" t="s">
         <v>127</v>
       </c>
@@ -5830,14 +5861,488 @@
       </c>
       <c r="C24" s="34"/>
       <c r="D24" s="34"/>
-      <c r="E24" s="35" t="s">
+      <c r="E24" s="34"/>
+      <c r="F24" s="35" t="s">
+        <v>401</v>
+      </c>
+      <c r="G24" s="35" t="s">
         <v>402</v>
       </c>
-      <c r="F24" s="35" t="s">
+      <c r="H24" s="35" t="s">
         <v>403</v>
       </c>
-      <c r="G24" s="35" t="s">
-        <v>404</v>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B66" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C66" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="B67" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C67" s="11" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -6138,10 +6643,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B15F685-1533-4446-BC92-30DBE05F964F}">
-  <dimension ref="A1:L119"/>
+  <dimension ref="A1:U119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="F75" sqref="F75"/>
+    <sheetView topLeftCell="A28" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6153,7 +6658,7 @@
     <col min="5" max="5" width="23" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="50" t="s">
         <v>53</v>
       </c>
@@ -6167,10 +6672,19 @@
         <v>33</v>
       </c>
       <c r="E1" s="50" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+        <v>404</v>
+      </c>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="58"/>
+      <c r="U1" s="58"/>
+    </row>
+    <row r="2" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>177</v>
       </c>
@@ -6193,8 +6707,17 @@
       <c r="J2" s="51"/>
       <c r="K2" s="51"/>
       <c r="L2" s="51"/>
-    </row>
-    <row r="3" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="59"/>
+      <c r="R2" s="59"/>
+      <c r="S2" s="59"/>
+      <c r="T2" s="59"/>
+      <c r="U2" s="59"/>
+    </row>
+    <row r="3" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>178</v>
       </c>
@@ -6217,8 +6740,17 @@
       <c r="J3" s="51"/>
       <c r="K3" s="51"/>
       <c r="L3" s="51"/>
-    </row>
-    <row r="4" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="59"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="59"/>
+      <c r="R3" s="59"/>
+      <c r="S3" s="59"/>
+      <c r="T3" s="59"/>
+      <c r="U3" s="59"/>
+    </row>
+    <row r="4" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>179</v>
       </c>
@@ -6241,8 +6773,17 @@
       <c r="J4" s="51"/>
       <c r="K4" s="51"/>
       <c r="L4" s="51"/>
-    </row>
-    <row r="5" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M4" s="59"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="59"/>
+      <c r="Q4" s="59"/>
+      <c r="R4" s="59"/>
+      <c r="S4" s="59"/>
+      <c r="T4" s="59"/>
+      <c r="U4" s="59"/>
+    </row>
+    <row r="5" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>180</v>
       </c>
@@ -6265,8 +6806,17 @@
       <c r="J5" s="51"/>
       <c r="K5" s="51"/>
       <c r="L5" s="51"/>
-    </row>
-    <row r="6" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M5" s="59"/>
+      <c r="N5" s="59"/>
+      <c r="O5" s="59"/>
+      <c r="P5" s="59"/>
+      <c r="Q5" s="59"/>
+      <c r="R5" s="59"/>
+      <c r="S5" s="59"/>
+      <c r="T5" s="59"/>
+      <c r="U5" s="59"/>
+    </row>
+    <row r="6" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>181</v>
       </c>
@@ -6289,8 +6839,17 @@
       <c r="J6" s="51"/>
       <c r="K6" s="51"/>
       <c r="L6" s="51"/>
-    </row>
-    <row r="7" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M6" s="59"/>
+      <c r="N6" s="59"/>
+      <c r="O6" s="59"/>
+      <c r="P6" s="59"/>
+      <c r="Q6" s="59"/>
+      <c r="R6" s="59"/>
+      <c r="S6" s="59"/>
+      <c r="T6" s="59"/>
+      <c r="U6" s="59"/>
+    </row>
+    <row r="7" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>182</v>
       </c>
@@ -6313,8 +6872,17 @@
       <c r="J7" s="51"/>
       <c r="K7" s="51"/>
       <c r="L7" s="51"/>
-    </row>
-    <row r="8" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M7" s="59"/>
+      <c r="N7" s="59"/>
+      <c r="O7" s="59"/>
+      <c r="P7" s="59"/>
+      <c r="Q7" s="59"/>
+      <c r="R7" s="59"/>
+      <c r="S7" s="59"/>
+      <c r="T7" s="59"/>
+      <c r="U7" s="59"/>
+    </row>
+    <row r="8" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>183</v>
       </c>
@@ -6337,8 +6905,17 @@
       <c r="J8" s="51"/>
       <c r="K8" s="51"/>
       <c r="L8" s="51"/>
-    </row>
-    <row r="9" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M8" s="59"/>
+      <c r="N8" s="59"/>
+      <c r="O8" s="59"/>
+      <c r="P8" s="59"/>
+      <c r="Q8" s="59"/>
+      <c r="R8" s="59"/>
+      <c r="S8" s="59"/>
+      <c r="T8" s="59"/>
+      <c r="U8" s="59"/>
+    </row>
+    <row r="9" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>184</v>
       </c>
@@ -6361,8 +6938,17 @@
       <c r="J9" s="51"/>
       <c r="K9" s="51"/>
       <c r="L9" s="51"/>
-    </row>
-    <row r="10" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M9" s="59"/>
+      <c r="N9" s="59"/>
+      <c r="O9" s="59"/>
+      <c r="P9" s="59"/>
+      <c r="Q9" s="59"/>
+      <c r="R9" s="59"/>
+      <c r="S9" s="59"/>
+      <c r="T9" s="59"/>
+      <c r="U9" s="59"/>
+    </row>
+    <row r="10" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>185</v>
       </c>
@@ -6385,8 +6971,17 @@
       <c r="J10" s="51"/>
       <c r="K10" s="51"/>
       <c r="L10" s="51"/>
-    </row>
-    <row r="11" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M10" s="59"/>
+      <c r="N10" s="59"/>
+      <c r="O10" s="59"/>
+      <c r="P10" s="59"/>
+      <c r="Q10" s="59"/>
+      <c r="R10" s="59"/>
+      <c r="S10" s="59"/>
+      <c r="T10" s="59"/>
+      <c r="U10" s="59"/>
+    </row>
+    <row r="11" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>186</v>
       </c>
@@ -6409,8 +7004,17 @@
       <c r="J11" s="51"/>
       <c r="K11" s="51"/>
       <c r="L11" s="51"/>
-    </row>
-    <row r="12" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M11" s="59"/>
+      <c r="N11" s="59"/>
+      <c r="O11" s="59"/>
+      <c r="P11" s="59"/>
+      <c r="Q11" s="59"/>
+      <c r="R11" s="59"/>
+      <c r="S11" s="59"/>
+      <c r="T11" s="59"/>
+      <c r="U11" s="59"/>
+    </row>
+    <row r="12" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>187</v>
       </c>
@@ -6433,8 +7037,17 @@
       <c r="J12" s="51"/>
       <c r="K12" s="51"/>
       <c r="L12" s="51"/>
-    </row>
-    <row r="13" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M12" s="59"/>
+      <c r="N12" s="59"/>
+      <c r="O12" s="59"/>
+      <c r="P12" s="59"/>
+      <c r="Q12" s="59"/>
+      <c r="R12" s="59"/>
+      <c r="S12" s="59"/>
+      <c r="T12" s="59"/>
+      <c r="U12" s="59"/>
+    </row>
+    <row r="13" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>188</v>
       </c>
@@ -6457,8 +7070,17 @@
       <c r="J13" s="51"/>
       <c r="K13" s="51"/>
       <c r="L13" s="51"/>
-    </row>
-    <row r="14" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M13" s="59"/>
+      <c r="N13" s="59"/>
+      <c r="O13" s="59"/>
+      <c r="P13" s="59"/>
+      <c r="Q13" s="59"/>
+      <c r="R13" s="59"/>
+      <c r="S13" s="59"/>
+      <c r="T13" s="59"/>
+      <c r="U13" s="59"/>
+    </row>
+    <row r="14" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>189</v>
       </c>
@@ -6481,8 +7103,17 @@
       <c r="J14" s="51"/>
       <c r="K14" s="51"/>
       <c r="L14" s="51"/>
-    </row>
-    <row r="15" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M14" s="59"/>
+      <c r="N14" s="59"/>
+      <c r="O14" s="59"/>
+      <c r="P14" s="59"/>
+      <c r="Q14" s="59"/>
+      <c r="R14" s="59"/>
+      <c r="S14" s="59"/>
+      <c r="T14" s="59"/>
+      <c r="U14" s="59"/>
+    </row>
+    <row r="15" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>190</v>
       </c>
@@ -6505,8 +7136,17 @@
       <c r="J15" s="51"/>
       <c r="K15" s="51"/>
       <c r="L15" s="51"/>
-    </row>
-    <row r="16" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M15" s="59"/>
+      <c r="N15" s="59"/>
+      <c r="O15" s="59"/>
+      <c r="P15" s="59"/>
+      <c r="Q15" s="59"/>
+      <c r="R15" s="59"/>
+      <c r="S15" s="59"/>
+      <c r="T15" s="59"/>
+      <c r="U15" s="59"/>
+    </row>
+    <row r="16" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>191</v>
       </c>
@@ -6529,8 +7169,17 @@
       <c r="J16" s="51"/>
       <c r="K16" s="51"/>
       <c r="L16" s="51"/>
-    </row>
-    <row r="17" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M16" s="59"/>
+      <c r="N16" s="59"/>
+      <c r="O16" s="59"/>
+      <c r="P16" s="59"/>
+      <c r="Q16" s="59"/>
+      <c r="R16" s="59"/>
+      <c r="S16" s="59"/>
+      <c r="T16" s="59"/>
+      <c r="U16" s="59"/>
+    </row>
+    <row r="17" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>285</v>
       </c>
@@ -6553,8 +7202,17 @@
       <c r="J17" s="51"/>
       <c r="K17" s="51"/>
       <c r="L17" s="51"/>
-    </row>
-    <row r="18" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M17" s="59"/>
+      <c r="N17" s="59"/>
+      <c r="O17" s="59"/>
+      <c r="P17" s="59"/>
+      <c r="Q17" s="59"/>
+      <c r="R17" s="59"/>
+      <c r="S17" s="59"/>
+      <c r="T17" s="59"/>
+      <c r="U17" s="59"/>
+    </row>
+    <row r="18" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>286</v>
       </c>
@@ -6568,7 +7226,7 @@
         <v>79</v>
       </c>
       <c r="E18" s="44" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="F18" s="51"/>
       <c r="G18" s="51"/>
@@ -6577,8 +7235,17 @@
       <c r="J18" s="51"/>
       <c r="K18" s="51"/>
       <c r="L18" s="51"/>
-    </row>
-    <row r="19" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M18" s="59"/>
+      <c r="N18" s="59"/>
+      <c r="O18" s="59"/>
+      <c r="P18" s="59"/>
+      <c r="Q18" s="59"/>
+      <c r="R18" s="59"/>
+      <c r="S18" s="59"/>
+      <c r="T18" s="59"/>
+      <c r="U18" s="59"/>
+    </row>
+    <row r="19" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>287</v>
       </c>
@@ -6592,7 +7259,7 @@
         <v>48</v>
       </c>
       <c r="E19" s="44" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="F19" s="51"/>
       <c r="G19" s="51"/>
@@ -6601,8 +7268,17 @@
       <c r="J19" s="51"/>
       <c r="K19" s="51"/>
       <c r="L19" s="51"/>
-    </row>
-    <row r="20" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M19" s="59"/>
+      <c r="N19" s="59"/>
+      <c r="O19" s="59"/>
+      <c r="P19" s="59"/>
+      <c r="Q19" s="59"/>
+      <c r="R19" s="59"/>
+      <c r="S19" s="59"/>
+      <c r="T19" s="59"/>
+      <c r="U19" s="59"/>
+    </row>
+    <row r="20" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>288</v>
       </c>
@@ -6616,7 +7292,7 @@
         <v>35</v>
       </c>
       <c r="E20" s="44" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="F20" s="51"/>
       <c r="G20" s="51"/>
@@ -6625,8 +7301,17 @@
       <c r="J20" s="51"/>
       <c r="K20" s="51"/>
       <c r="L20" s="51"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M20" s="59"/>
+      <c r="N20" s="59"/>
+      <c r="O20" s="59"/>
+      <c r="P20" s="59"/>
+      <c r="Q20" s="59"/>
+      <c r="R20" s="59"/>
+      <c r="S20" s="59"/>
+      <c r="T20" s="59"/>
+      <c r="U20" s="59"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>176</v>
       </c>
@@ -6638,8 +7323,17 @@
       <c r="J21" s="51"/>
       <c r="K21" s="51"/>
       <c r="L21" s="51"/>
-    </row>
-    <row r="22" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M21" s="59"/>
+      <c r="N21" s="59"/>
+      <c r="O21" s="59"/>
+      <c r="P21" s="59"/>
+      <c r="Q21" s="59"/>
+      <c r="R21" s="59"/>
+      <c r="S21" s="59"/>
+      <c r="T21" s="59"/>
+      <c r="U21" s="59"/>
+    </row>
+    <row r="22" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>192</v>
       </c>
@@ -6662,8 +7356,17 @@
       <c r="J22" s="51"/>
       <c r="K22" s="51"/>
       <c r="L22" s="51"/>
-    </row>
-    <row r="23" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M22" s="59"/>
+      <c r="N22" s="59"/>
+      <c r="O22" s="59"/>
+      <c r="P22" s="59"/>
+      <c r="Q22" s="59"/>
+      <c r="R22" s="59"/>
+      <c r="S22" s="59"/>
+      <c r="T22" s="59"/>
+      <c r="U22" s="59"/>
+    </row>
+    <row r="23" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>193</v>
       </c>
@@ -6686,8 +7389,17 @@
       <c r="J23" s="51"/>
       <c r="K23" s="51"/>
       <c r="L23" s="51"/>
-    </row>
-    <row r="24" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M23" s="59"/>
+      <c r="N23" s="59"/>
+      <c r="O23" s="59"/>
+      <c r="P23" s="59"/>
+      <c r="Q23" s="59"/>
+      <c r="R23" s="59"/>
+      <c r="S23" s="59"/>
+      <c r="T23" s="59"/>
+      <c r="U23" s="59"/>
+    </row>
+    <row r="24" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>194</v>
       </c>
@@ -6710,8 +7422,17 @@
       <c r="J24" s="51"/>
       <c r="K24" s="51"/>
       <c r="L24" s="51"/>
-    </row>
-    <row r="25" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M24" s="59"/>
+      <c r="N24" s="59"/>
+      <c r="O24" s="59"/>
+      <c r="P24" s="59"/>
+      <c r="Q24" s="59"/>
+      <c r="R24" s="59"/>
+      <c r="S24" s="59"/>
+      <c r="T24" s="59"/>
+      <c r="U24" s="59"/>
+    </row>
+    <row r="25" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>195</v>
       </c>
@@ -6734,8 +7455,17 @@
       <c r="J25" s="51"/>
       <c r="K25" s="51"/>
       <c r="L25" s="51"/>
-    </row>
-    <row r="26" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M25" s="59"/>
+      <c r="N25" s="59"/>
+      <c r="O25" s="59"/>
+      <c r="P25" s="59"/>
+      <c r="Q25" s="59"/>
+      <c r="R25" s="59"/>
+      <c r="S25" s="59"/>
+      <c r="T25" s="59"/>
+      <c r="U25" s="59"/>
+    </row>
+    <row r="26" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>289</v>
       </c>
@@ -6758,8 +7488,17 @@
       <c r="J26" s="51"/>
       <c r="K26" s="51"/>
       <c r="L26" s="51"/>
-    </row>
-    <row r="27" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M26" s="59"/>
+      <c r="N26" s="59"/>
+      <c r="O26" s="59"/>
+      <c r="P26" s="59"/>
+      <c r="Q26" s="59"/>
+      <c r="R26" s="59"/>
+      <c r="S26" s="59"/>
+      <c r="T26" s="59"/>
+      <c r="U26" s="59"/>
+    </row>
+    <row r="27" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>290</v>
       </c>
@@ -6782,8 +7521,17 @@
       <c r="J27" s="51"/>
       <c r="K27" s="51"/>
       <c r="L27" s="51"/>
-    </row>
-    <row r="28" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M27" s="59"/>
+      <c r="N27" s="59"/>
+      <c r="O27" s="59"/>
+      <c r="P27" s="59"/>
+      <c r="Q27" s="59"/>
+      <c r="R27" s="59"/>
+      <c r="S27" s="59"/>
+      <c r="T27" s="59"/>
+      <c r="U27" s="59"/>
+    </row>
+    <row r="28" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>196</v>
       </c>
@@ -6806,8 +7554,17 @@
       <c r="J28" s="51"/>
       <c r="K28" s="51"/>
       <c r="L28" s="51"/>
-    </row>
-    <row r="29" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M28" s="59"/>
+      <c r="N28" s="59"/>
+      <c r="O28" s="59"/>
+      <c r="P28" s="59"/>
+      <c r="Q28" s="59"/>
+      <c r="R28" s="59"/>
+      <c r="S28" s="59"/>
+      <c r="T28" s="59"/>
+      <c r="U28" s="59"/>
+    </row>
+    <row r="29" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
         <v>197</v>
       </c>
@@ -6830,8 +7587,17 @@
       <c r="J29" s="51"/>
       <c r="K29" s="51"/>
       <c r="L29" s="51"/>
-    </row>
-    <row r="30" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M29" s="59"/>
+      <c r="N29" s="59"/>
+      <c r="O29" s="59"/>
+      <c r="P29" s="59"/>
+      <c r="Q29" s="59"/>
+      <c r="R29" s="59"/>
+      <c r="S29" s="59"/>
+      <c r="T29" s="59"/>
+      <c r="U29" s="59"/>
+    </row>
+    <row r="30" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
         <v>198</v>
       </c>
@@ -6854,8 +7620,17 @@
       <c r="J30" s="51"/>
       <c r="K30" s="51"/>
       <c r="L30" s="51"/>
-    </row>
-    <row r="31" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M30" s="59"/>
+      <c r="N30" s="59"/>
+      <c r="O30" s="59"/>
+      <c r="P30" s="59"/>
+      <c r="Q30" s="59"/>
+      <c r="R30" s="59"/>
+      <c r="S30" s="59"/>
+      <c r="T30" s="59"/>
+      <c r="U30" s="59"/>
+    </row>
+    <row r="31" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>199</v>
       </c>
@@ -6878,8 +7653,17 @@
       <c r="J31" s="51"/>
       <c r="K31" s="51"/>
       <c r="L31" s="51"/>
-    </row>
-    <row r="32" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M31" s="59"/>
+      <c r="N31" s="59"/>
+      <c r="O31" s="59"/>
+      <c r="P31" s="59"/>
+      <c r="Q31" s="59"/>
+      <c r="R31" s="59"/>
+      <c r="S31" s="59"/>
+      <c r="T31" s="59"/>
+      <c r="U31" s="59"/>
+    </row>
+    <row r="32" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>200</v>
       </c>
@@ -6902,8 +7686,17 @@
       <c r="J32" s="51"/>
       <c r="K32" s="51"/>
       <c r="L32" s="51"/>
-    </row>
-    <row r="33" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M32" s="59"/>
+      <c r="N32" s="59"/>
+      <c r="O32" s="59"/>
+      <c r="P32" s="59"/>
+      <c r="Q32" s="59"/>
+      <c r="R32" s="59"/>
+      <c r="S32" s="59"/>
+      <c r="T32" s="59"/>
+      <c r="U32" s="59"/>
+    </row>
+    <row r="33" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
         <v>201</v>
       </c>
@@ -6926,8 +7719,17 @@
       <c r="J33" s="51"/>
       <c r="K33" s="51"/>
       <c r="L33" s="51"/>
-    </row>
-    <row r="34" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M33" s="59"/>
+      <c r="N33" s="59"/>
+      <c r="O33" s="59"/>
+      <c r="P33" s="59"/>
+      <c r="Q33" s="59"/>
+      <c r="R33" s="59"/>
+      <c r="S33" s="59"/>
+      <c r="T33" s="59"/>
+      <c r="U33" s="59"/>
+    </row>
+    <row r="34" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
         <v>202</v>
       </c>
@@ -6950,8 +7752,17 @@
       <c r="J34" s="51"/>
       <c r="K34" s="51"/>
       <c r="L34" s="51"/>
-    </row>
-    <row r="35" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M34" s="59"/>
+      <c r="N34" s="59"/>
+      <c r="O34" s="59"/>
+      <c r="P34" s="59"/>
+      <c r="Q34" s="59"/>
+      <c r="R34" s="59"/>
+      <c r="S34" s="59"/>
+      <c r="T34" s="59"/>
+      <c r="U34" s="59"/>
+    </row>
+    <row r="35" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
         <v>203</v>
       </c>
@@ -6974,8 +7785,17 @@
       <c r="J35" s="51"/>
       <c r="K35" s="51"/>
       <c r="L35" s="51"/>
-    </row>
-    <row r="36" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M35" s="59"/>
+      <c r="N35" s="59"/>
+      <c r="O35" s="59"/>
+      <c r="P35" s="59"/>
+      <c r="Q35" s="59"/>
+      <c r="R35" s="59"/>
+      <c r="S35" s="59"/>
+      <c r="T35" s="59"/>
+      <c r="U35" s="59"/>
+    </row>
+    <row r="36" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>204</v>
       </c>
@@ -6998,8 +7818,17 @@
       <c r="J36" s="51"/>
       <c r="K36" s="51"/>
       <c r="L36" s="51"/>
-    </row>
-    <row r="37" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M36" s="59"/>
+      <c r="N36" s="59"/>
+      <c r="O36" s="59"/>
+      <c r="P36" s="59"/>
+      <c r="Q36" s="59"/>
+      <c r="R36" s="59"/>
+      <c r="S36" s="59"/>
+      <c r="T36" s="59"/>
+      <c r="U36" s="59"/>
+    </row>
+    <row r="37" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
         <v>205</v>
       </c>
@@ -7022,8 +7851,17 @@
       <c r="J37" s="51"/>
       <c r="K37" s="51"/>
       <c r="L37" s="51"/>
-    </row>
-    <row r="38" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M37" s="59"/>
+      <c r="N37" s="59"/>
+      <c r="O37" s="59"/>
+      <c r="P37" s="59"/>
+      <c r="Q37" s="59"/>
+      <c r="R37" s="59"/>
+      <c r="S37" s="59"/>
+      <c r="T37" s="59"/>
+      <c r="U37" s="59"/>
+    </row>
+    <row r="38" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
         <v>206</v>
       </c>
@@ -7046,8 +7884,17 @@
       <c r="J38" s="51"/>
       <c r="K38" s="51"/>
       <c r="L38" s="51"/>
-    </row>
-    <row r="39" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M38" s="59"/>
+      <c r="N38" s="59"/>
+      <c r="O38" s="59"/>
+      <c r="P38" s="59"/>
+      <c r="Q38" s="59"/>
+      <c r="R38" s="59"/>
+      <c r="S38" s="59"/>
+      <c r="T38" s="59"/>
+      <c r="U38" s="59"/>
+    </row>
+    <row r="39" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
         <v>207</v>
       </c>
@@ -7070,8 +7917,17 @@
       <c r="J39" s="51"/>
       <c r="K39" s="51"/>
       <c r="L39" s="51"/>
-    </row>
-    <row r="40" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M39" s="59"/>
+      <c r="N39" s="59"/>
+      <c r="O39" s="59"/>
+      <c r="P39" s="59"/>
+      <c r="Q39" s="59"/>
+      <c r="R39" s="59"/>
+      <c r="S39" s="59"/>
+      <c r="T39" s="59"/>
+      <c r="U39" s="59"/>
+    </row>
+    <row r="40" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
         <v>208</v>
       </c>
@@ -7094,8 +7950,17 @@
       <c r="J40" s="51"/>
       <c r="K40" s="51"/>
       <c r="L40" s="51"/>
-    </row>
-    <row r="41" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M40" s="59"/>
+      <c r="N40" s="59"/>
+      <c r="O40" s="59"/>
+      <c r="P40" s="59"/>
+      <c r="Q40" s="59"/>
+      <c r="R40" s="59"/>
+      <c r="S40" s="59"/>
+      <c r="T40" s="59"/>
+      <c r="U40" s="59"/>
+    </row>
+    <row r="41" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
         <v>209</v>
       </c>
@@ -7118,8 +7983,17 @@
       <c r="J41" s="51"/>
       <c r="K41" s="51"/>
       <c r="L41" s="51"/>
-    </row>
-    <row r="42" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M41" s="59"/>
+      <c r="N41" s="59"/>
+      <c r="O41" s="59"/>
+      <c r="P41" s="59"/>
+      <c r="Q41" s="59"/>
+      <c r="R41" s="59"/>
+      <c r="S41" s="59"/>
+      <c r="T41" s="59"/>
+      <c r="U41" s="59"/>
+    </row>
+    <row r="42" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
         <v>210</v>
       </c>
@@ -7142,8 +8016,17 @@
       <c r="J42" s="51"/>
       <c r="K42" s="51"/>
       <c r="L42" s="51"/>
-    </row>
-    <row r="43" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M42" s="59"/>
+      <c r="N42" s="59"/>
+      <c r="O42" s="59"/>
+      <c r="P42" s="59"/>
+      <c r="Q42" s="59"/>
+      <c r="R42" s="59"/>
+      <c r="S42" s="59"/>
+      <c r="T42" s="59"/>
+      <c r="U42" s="59"/>
+    </row>
+    <row r="43" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
         <v>211</v>
       </c>
@@ -7166,8 +8049,17 @@
       <c r="J43" s="51"/>
       <c r="K43" s="51"/>
       <c r="L43" s="51"/>
-    </row>
-    <row r="44" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M43" s="59"/>
+      <c r="N43" s="59"/>
+      <c r="O43" s="59"/>
+      <c r="P43" s="59"/>
+      <c r="Q43" s="59"/>
+      <c r="R43" s="59"/>
+      <c r="S43" s="59"/>
+      <c r="T43" s="59"/>
+      <c r="U43" s="59"/>
+    </row>
+    <row r="44" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
         <v>212</v>
       </c>
@@ -7190,8 +8082,17 @@
       <c r="J44" s="51"/>
       <c r="K44" s="51"/>
       <c r="L44" s="51"/>
-    </row>
-    <row r="45" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M44" s="59"/>
+      <c r="N44" s="59"/>
+      <c r="O44" s="59"/>
+      <c r="P44" s="59"/>
+      <c r="Q44" s="59"/>
+      <c r="R44" s="59"/>
+      <c r="S44" s="59"/>
+      <c r="T44" s="59"/>
+      <c r="U44" s="59"/>
+    </row>
+    <row r="45" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
         <v>291</v>
       </c>
@@ -7205,7 +8106,7 @@
         <v>278</v>
       </c>
       <c r="E45" s="44" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="F45" s="51"/>
       <c r="G45" s="51"/>
@@ -7214,8 +8115,17 @@
       <c r="J45" s="51"/>
       <c r="K45" s="51"/>
       <c r="L45" s="51"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M45" s="59"/>
+      <c r="N45" s="59"/>
+      <c r="O45" s="59"/>
+      <c r="P45" s="59"/>
+      <c r="Q45" s="59"/>
+      <c r="R45" s="59"/>
+      <c r="S45" s="59"/>
+      <c r="T45" s="59"/>
+      <c r="U45" s="59"/>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>176</v>
       </c>
@@ -7227,8 +8137,17 @@
       <c r="J46" s="51"/>
       <c r="K46" s="51"/>
       <c r="L46" s="51"/>
-    </row>
-    <row r="47" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M46" s="59"/>
+      <c r="N46" s="59"/>
+      <c r="O46" s="59"/>
+      <c r="P46" s="59"/>
+      <c r="Q46" s="59"/>
+      <c r="R46" s="59"/>
+      <c r="S46" s="59"/>
+      <c r="T46" s="59"/>
+      <c r="U46" s="59"/>
+    </row>
+    <row r="47" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="20" t="s">
         <v>213</v>
       </c>
@@ -7251,8 +8170,17 @@
       <c r="J47" s="51"/>
       <c r="K47" s="51"/>
       <c r="L47" s="51"/>
-    </row>
-    <row r="48" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M47" s="59"/>
+      <c r="N47" s="59"/>
+      <c r="O47" s="59"/>
+      <c r="P47" s="59"/>
+      <c r="Q47" s="59"/>
+      <c r="R47" s="59"/>
+      <c r="S47" s="59"/>
+      <c r="T47" s="59"/>
+      <c r="U47" s="59"/>
+    </row>
+    <row r="48" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
         <v>214</v>
       </c>
@@ -7275,8 +8203,17 @@
       <c r="J48" s="51"/>
       <c r="K48" s="51"/>
       <c r="L48" s="51"/>
-    </row>
-    <row r="49" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M48" s="59"/>
+      <c r="N48" s="59"/>
+      <c r="O48" s="59"/>
+      <c r="P48" s="59"/>
+      <c r="Q48" s="59"/>
+      <c r="R48" s="59"/>
+      <c r="S48" s="59"/>
+      <c r="T48" s="59"/>
+      <c r="U48" s="59"/>
+    </row>
+    <row r="49" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="20" t="s">
         <v>215</v>
       </c>
@@ -7299,8 +8236,17 @@
       <c r="J49" s="51"/>
       <c r="K49" s="51"/>
       <c r="L49" s="51"/>
-    </row>
-    <row r="50" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M49" s="59"/>
+      <c r="N49" s="59"/>
+      <c r="O49" s="59"/>
+      <c r="P49" s="59"/>
+      <c r="Q49" s="59"/>
+      <c r="R49" s="59"/>
+      <c r="S49" s="59"/>
+      <c r="T49" s="59"/>
+      <c r="U49" s="59"/>
+    </row>
+    <row r="50" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
         <v>216</v>
       </c>
@@ -7323,8 +8269,17 @@
       <c r="J50" s="51"/>
       <c r="K50" s="51"/>
       <c r="L50" s="51"/>
-    </row>
-    <row r="51" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M50" s="59"/>
+      <c r="N50" s="59"/>
+      <c r="O50" s="59"/>
+      <c r="P50" s="59"/>
+      <c r="Q50" s="59"/>
+      <c r="R50" s="59"/>
+      <c r="S50" s="59"/>
+      <c r="T50" s="59"/>
+      <c r="U50" s="59"/>
+    </row>
+    <row r="51" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
         <v>217</v>
       </c>
@@ -7347,8 +8302,17 @@
       <c r="J51" s="51"/>
       <c r="K51" s="51"/>
       <c r="L51" s="51"/>
-    </row>
-    <row r="52" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M51" s="59"/>
+      <c r="N51" s="59"/>
+      <c r="O51" s="59"/>
+      <c r="P51" s="59"/>
+      <c r="Q51" s="59"/>
+      <c r="R51" s="59"/>
+      <c r="S51" s="59"/>
+      <c r="T51" s="59"/>
+      <c r="U51" s="59"/>
+    </row>
+    <row r="52" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
         <v>218</v>
       </c>
@@ -7371,8 +8335,17 @@
       <c r="J52" s="51"/>
       <c r="K52" s="51"/>
       <c r="L52" s="51"/>
-    </row>
-    <row r="53" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M52" s="59"/>
+      <c r="N52" s="59"/>
+      <c r="O52" s="59"/>
+      <c r="P52" s="59"/>
+      <c r="Q52" s="59"/>
+      <c r="R52" s="59"/>
+      <c r="S52" s="59"/>
+      <c r="T52" s="59"/>
+      <c r="U52" s="59"/>
+    </row>
+    <row r="53" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="20" t="s">
         <v>219</v>
       </c>
@@ -7395,8 +8368,17 @@
       <c r="J53" s="51"/>
       <c r="K53" s="51"/>
       <c r="L53" s="51"/>
-    </row>
-    <row r="54" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M53" s="59"/>
+      <c r="N53" s="59"/>
+      <c r="O53" s="59"/>
+      <c r="P53" s="59"/>
+      <c r="Q53" s="59"/>
+      <c r="R53" s="59"/>
+      <c r="S53" s="59"/>
+      <c r="T53" s="59"/>
+      <c r="U53" s="59"/>
+    </row>
+    <row r="54" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
         <v>220</v>
       </c>
@@ -7419,8 +8401,17 @@
       <c r="J54" s="51"/>
       <c r="K54" s="51"/>
       <c r="L54" s="51"/>
-    </row>
-    <row r="55" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M54" s="59"/>
+      <c r="N54" s="59"/>
+      <c r="O54" s="59"/>
+      <c r="P54" s="59"/>
+      <c r="Q54" s="59"/>
+      <c r="R54" s="59"/>
+      <c r="S54" s="59"/>
+      <c r="T54" s="59"/>
+      <c r="U54" s="59"/>
+    </row>
+    <row r="55" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="20" t="s">
         <v>221</v>
       </c>
@@ -7443,8 +8434,17 @@
       <c r="J55" s="51"/>
       <c r="K55" s="51"/>
       <c r="L55" s="51"/>
-    </row>
-    <row r="56" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M55" s="59"/>
+      <c r="N55" s="59"/>
+      <c r="O55" s="59"/>
+      <c r="P55" s="59"/>
+      <c r="Q55" s="59"/>
+      <c r="R55" s="59"/>
+      <c r="S55" s="59"/>
+      <c r="T55" s="59"/>
+      <c r="U55" s="59"/>
+    </row>
+    <row r="56" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="20" t="s">
         <v>222</v>
       </c>
@@ -7467,8 +8467,17 @@
       <c r="J56" s="51"/>
       <c r="K56" s="51"/>
       <c r="L56" s="51"/>
-    </row>
-    <row r="57" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M56" s="59"/>
+      <c r="N56" s="59"/>
+      <c r="O56" s="59"/>
+      <c r="P56" s="59"/>
+      <c r="Q56" s="59"/>
+      <c r="R56" s="59"/>
+      <c r="S56" s="59"/>
+      <c r="T56" s="59"/>
+      <c r="U56" s="59"/>
+    </row>
+    <row r="57" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="20" t="s">
         <v>223</v>
       </c>
@@ -7491,8 +8500,17 @@
       <c r="J57" s="51"/>
       <c r="K57" s="51"/>
       <c r="L57" s="51"/>
-    </row>
-    <row r="58" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M57" s="59"/>
+      <c r="N57" s="59"/>
+      <c r="O57" s="59"/>
+      <c r="P57" s="59"/>
+      <c r="Q57" s="59"/>
+      <c r="R57" s="59"/>
+      <c r="S57" s="59"/>
+      <c r="T57" s="59"/>
+      <c r="U57" s="59"/>
+    </row>
+    <row r="58" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="20" t="s">
         <v>224</v>
       </c>
@@ -7515,8 +8533,17 @@
       <c r="J58" s="51"/>
       <c r="K58" s="51"/>
       <c r="L58" s="51"/>
-    </row>
-    <row r="59" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M58" s="59"/>
+      <c r="N58" s="59"/>
+      <c r="O58" s="59"/>
+      <c r="P58" s="59"/>
+      <c r="Q58" s="59"/>
+      <c r="R58" s="59"/>
+      <c r="S58" s="59"/>
+      <c r="T58" s="59"/>
+      <c r="U58" s="59"/>
+    </row>
+    <row r="59" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="20" t="s">
         <v>225</v>
       </c>
@@ -7539,8 +8566,17 @@
       <c r="J59" s="51"/>
       <c r="K59" s="51"/>
       <c r="L59" s="51"/>
-    </row>
-    <row r="60" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M59" s="59"/>
+      <c r="N59" s="59"/>
+      <c r="O59" s="59"/>
+      <c r="P59" s="59"/>
+      <c r="Q59" s="59"/>
+      <c r="R59" s="59"/>
+      <c r="S59" s="59"/>
+      <c r="T59" s="59"/>
+      <c r="U59" s="59"/>
+    </row>
+    <row r="60" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="20" t="s">
         <v>226</v>
       </c>
@@ -7563,8 +8599,17 @@
       <c r="J60" s="51"/>
       <c r="K60" s="51"/>
       <c r="L60" s="51"/>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M60" s="59"/>
+      <c r="N60" s="59"/>
+      <c r="O60" s="59"/>
+      <c r="P60" s="59"/>
+      <c r="Q60" s="59"/>
+      <c r="R60" s="59"/>
+      <c r="S60" s="59"/>
+      <c r="T60" s="59"/>
+      <c r="U60" s="59"/>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>176</v>
       </c>
@@ -7576,8 +8621,17 @@
       <c r="J61" s="51"/>
       <c r="K61" s="51"/>
       <c r="L61" s="51"/>
-    </row>
-    <row r="62" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M61" s="59"/>
+      <c r="N61" s="59"/>
+      <c r="O61" s="59"/>
+      <c r="P61" s="59"/>
+      <c r="Q61" s="59"/>
+      <c r="R61" s="59"/>
+      <c r="S61" s="59"/>
+      <c r="T61" s="59"/>
+      <c r="U61" s="59"/>
+    </row>
+    <row r="62" spans="1:21" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="26" t="s">
         <v>227</v>
       </c>
@@ -7600,8 +8654,17 @@
       <c r="J62" s="51"/>
       <c r="K62" s="51"/>
       <c r="L62" s="51"/>
-    </row>
-    <row r="63" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M62" s="59"/>
+      <c r="N62" s="59"/>
+      <c r="O62" s="59"/>
+      <c r="P62" s="59"/>
+      <c r="Q62" s="59"/>
+      <c r="R62" s="59"/>
+      <c r="S62" s="59"/>
+      <c r="T62" s="59"/>
+      <c r="U62" s="59"/>
+    </row>
+    <row r="63" spans="1:21" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="26" t="s">
         <v>228</v>
       </c>
@@ -7624,8 +8687,17 @@
       <c r="J63" s="51"/>
       <c r="K63" s="51"/>
       <c r="L63" s="51"/>
-    </row>
-    <row r="64" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M63" s="59"/>
+      <c r="N63" s="59"/>
+      <c r="O63" s="59"/>
+      <c r="P63" s="59"/>
+      <c r="Q63" s="59"/>
+      <c r="R63" s="59"/>
+      <c r="S63" s="59"/>
+      <c r="T63" s="59"/>
+      <c r="U63" s="59"/>
+    </row>
+    <row r="64" spans="1:21" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="26" t="s">
         <v>229</v>
       </c>
@@ -7648,8 +8720,17 @@
       <c r="J64" s="51"/>
       <c r="K64" s="51"/>
       <c r="L64" s="51"/>
-    </row>
-    <row r="65" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M64" s="59"/>
+      <c r="N64" s="59"/>
+      <c r="O64" s="59"/>
+      <c r="P64" s="59"/>
+      <c r="Q64" s="59"/>
+      <c r="R64" s="59"/>
+      <c r="S64" s="59"/>
+      <c r="T64" s="59"/>
+      <c r="U64" s="59"/>
+    </row>
+    <row r="65" spans="1:21" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="26" t="s">
         <v>230</v>
       </c>
@@ -7672,8 +8753,17 @@
       <c r="J65" s="51"/>
       <c r="K65" s="51"/>
       <c r="L65" s="51"/>
-    </row>
-    <row r="66" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M65" s="59"/>
+      <c r="N65" s="59"/>
+      <c r="O65" s="59"/>
+      <c r="P65" s="59"/>
+      <c r="Q65" s="59"/>
+      <c r="R65" s="59"/>
+      <c r="S65" s="59"/>
+      <c r="T65" s="59"/>
+      <c r="U65" s="59"/>
+    </row>
+    <row r="66" spans="1:21" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="26" t="s">
         <v>231</v>
       </c>
@@ -7696,8 +8786,17 @@
       <c r="J66" s="51"/>
       <c r="K66" s="51"/>
       <c r="L66" s="51"/>
-    </row>
-    <row r="67" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M66" s="59"/>
+      <c r="N66" s="59"/>
+      <c r="O66" s="59"/>
+      <c r="P66" s="59"/>
+      <c r="Q66" s="59"/>
+      <c r="R66" s="59"/>
+      <c r="S66" s="59"/>
+      <c r="T66" s="59"/>
+      <c r="U66" s="59"/>
+    </row>
+    <row r="67" spans="1:21" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="26" t="s">
         <v>232</v>
       </c>
@@ -7711,7 +8810,7 @@
         <v>45</v>
       </c>
       <c r="E67" s="44" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="F67" s="51"/>
       <c r="G67" s="51"/>
@@ -7720,8 +8819,17 @@
       <c r="J67" s="51"/>
       <c r="K67" s="51"/>
       <c r="L67" s="51"/>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M67" s="59"/>
+      <c r="N67" s="59"/>
+      <c r="O67" s="59"/>
+      <c r="P67" s="59"/>
+      <c r="Q67" s="59"/>
+      <c r="R67" s="59"/>
+      <c r="S67" s="59"/>
+      <c r="T67" s="59"/>
+      <c r="U67" s="59"/>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E68" s="44"/>
       <c r="F68" s="51"/>
       <c r="G68" s="51"/>
@@ -7731,7 +8839,7 @@
       <c r="K68" s="51"/>
       <c r="L68" s="51"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A69" s="16" t="s">
         <v>267</v>
       </c>
@@ -7755,7 +8863,7 @@
       <c r="K69" s="51"/>
       <c r="L69" s="51"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A70" s="16" t="s">
         <v>268</v>
       </c>
@@ -7779,7 +8887,7 @@
       <c r="K70" s="51"/>
       <c r="L70" s="51"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A71" s="16" t="s">
         <v>269</v>
       </c>
@@ -7803,7 +8911,7 @@
       <c r="K71" s="51"/>
       <c r="L71" s="51"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A72" s="16" t="s">
         <v>270</v>
       </c>
@@ -7827,7 +8935,7 @@
       <c r="K72" s="51"/>
       <c r="L72" s="51"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>271</v>
       </c>
@@ -7851,7 +8959,7 @@
       <c r="K73" s="51"/>
       <c r="L73" s="51"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>272</v>
       </c>
@@ -7875,7 +8983,7 @@
       <c r="K74" s="51"/>
       <c r="L74" s="51"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E75" s="44"/>
       <c r="F75" s="51"/>
       <c r="G75" s="51"/>
@@ -7885,7 +8993,7 @@
       <c r="K75" s="51"/>
       <c r="L75" s="51"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E76" s="44"/>
       <c r="F76" s="51"/>
       <c r="G76" s="51"/>
@@ -7895,7 +9003,7 @@
       <c r="K76" s="51"/>
       <c r="L76" s="51"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E77" s="44"/>
       <c r="F77" s="51"/>
       <c r="G77" s="51"/>
@@ -7905,7 +9013,7 @@
       <c r="K77" s="51"/>
       <c r="L77" s="51"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E78" s="44"/>
       <c r="F78" s="51"/>
       <c r="G78" s="51"/>
@@ -7915,7 +9023,7 @@
       <c r="K78" s="51"/>
       <c r="L78" s="51"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E79" s="44"/>
       <c r="F79" s="51"/>
       <c r="G79" s="51"/>
@@ -7925,7 +9033,7 @@
       <c r="K79" s="51"/>
       <c r="L79" s="51"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E80" s="44"/>
       <c r="F80" s="51"/>
       <c r="G80" s="51"/>
@@ -8346,12 +9454,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="0c85289e-a0a4-4193-8a36-83840327cccf" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="48f24ce9-3fee-408f-adaa-6c70c8fcad88">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8610,20 +9720,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="0c85289e-a0a4-4193-8a36-83840327cccf" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="48f24ce9-3fee-408f-adaa-6c70c8fcad88">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4B4AC16-F988-4D41-8F01-205FCE01B916}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{084C8915-1C39-4800-8751-2F69F55F51E7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="48f24ce9-3fee-408f-adaa-6c70c8fcad88"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="0c85289e-a0a4-4193-8a36-83840327cccf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8648,18 +9765,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{084C8915-1C39-4800-8751-2F69F55F51E7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4B4AC16-F988-4D41-8F01-205FCE01B916}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="48f24ce9-3fee-408f-adaa-6c70c8fcad88"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="0c85289e-a0a4-4193-8a36-83840327cccf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>